<commit_message>
Modified the IT 1A Grading sheet
</commit_message>
<xml_diff>
--- a/DCIT 21 - IT 1A/LEC AND LAB - IT 1A.xlsx
+++ b/DCIT 21 - IT 1A/LEC AND LAB - IT 1A.xlsx
@@ -2540,99 +2540,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2672,129 +2610,104 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2835,6 +2748,93 @@
     </xf>
     <xf numFmtId="9" fontId="32" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2893,6 +2893,102 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -2966,102 +3062,6 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5565,7 +5565,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5598,82 +5598,82 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18">
-      <c r="A2" s="135" t="s">
+      <c r="A2" s="167" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="135"/>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="135"/>
-      <c r="K2" s="135"/>
-      <c r="L2" s="135"/>
-      <c r="M2" s="135"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="135"/>
-      <c r="B3" s="135"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135"/>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="135"/>
+      <c r="A3" s="167"/>
+      <c r="B3" s="167"/>
+      <c r="C3" s="167"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="167"/>
+      <c r="F3" s="167"/>
+      <c r="G3" s="167"/>
+      <c r="H3" s="167"/>
+      <c r="I3" s="167"/>
+      <c r="J3" s="167"/>
+      <c r="K3" s="167"/>
+      <c r="L3" s="167"/>
+      <c r="M3" s="167"/>
     </row>
     <row r="4" spans="1:18" ht="16.5" customHeight="1">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="162" t="s">
         <v>114</v>
       </c>
-      <c r="B4" s="127"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="127"/>
-      <c r="E4" s="127"/>
-      <c r="F4" s="127"/>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="127"/>
-      <c r="K4" s="127"/>
-      <c r="L4" s="127"/>
-      <c r="M4" s="127"/>
+      <c r="B4" s="162"/>
+      <c r="C4" s="162"/>
+      <c r="D4" s="162"/>
+      <c r="E4" s="162"/>
+      <c r="F4" s="162"/>
+      <c r="G4" s="162"/>
+      <c r="H4" s="162"/>
+      <c r="I4" s="162"/>
+      <c r="J4" s="162"/>
+      <c r="K4" s="162"/>
+      <c r="L4" s="162"/>
+      <c r="M4" s="162"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A5" s="126"/>
-      <c r="B5" s="126"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="126"/>
-      <c r="E5" s="126"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="126"/>
-      <c r="H5" s="126"/>
-      <c r="I5" s="126"/>
-      <c r="J5" s="126"/>
-      <c r="K5" s="126"/>
-      <c r="L5" s="126"/>
-      <c r="M5" s="126"/>
+      <c r="A5" s="161"/>
+      <c r="B5" s="161"/>
+      <c r="C5" s="161"/>
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="161"/>
+      <c r="H5" s="161"/>
+      <c r="I5" s="161"/>
+      <c r="J5" s="161"/>
+      <c r="K5" s="161"/>
+      <c r="L5" s="161"/>
+      <c r="M5" s="161"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="164" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="165"/>
-      <c r="C6" s="166" t="s">
+      <c r="A6" s="126" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="127"/>
+      <c r="C6" s="128" t="s">
         <v>334</v>
       </c>
-      <c r="D6" s="166"/>
-      <c r="E6" s="167" t="s">
+      <c r="D6" s="128"/>
+      <c r="E6" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="167"/>
+      <c r="F6" s="129"/>
       <c r="G6" s="1">
         <v>2</v>
       </c>
@@ -5681,28 +5681,28 @@
         <v>2</v>
       </c>
       <c r="I6" s="1"/>
-      <c r="J6" s="168" t="s">
+      <c r="J6" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="168"/>
-      <c r="L6" s="169"/>
-      <c r="M6" s="169"/>
+      <c r="K6" s="130"/>
+      <c r="L6" s="131"/>
+      <c r="M6" s="131"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="170" t="s">
+      <c r="A7" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="171"/>
+      <c r="B7" s="133"/>
       <c r="C7" s="3" t="s">
         <v>335</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="172" t="s">
+      <c r="E7" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="172"/>
+      <c r="F7" s="134"/>
       <c r="G7" s="5">
         <v>1</v>
       </c>
@@ -5710,28 +5710,28 @@
         <v>7</v>
       </c>
       <c r="I7" s="7"/>
-      <c r="J7" s="172" t="s">
+      <c r="J7" s="134" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="172"/>
-      <c r="L7" s="173"/>
-      <c r="M7" s="173"/>
+      <c r="K7" s="134"/>
+      <c r="L7" s="135"/>
+      <c r="M7" s="135"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A8" s="152" t="s">
+      <c r="A8" s="136" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="153"/>
+      <c r="B8" s="137"/>
       <c r="C8" s="8" t="s">
         <v>336</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="E8" s="154" t="s">
+      <c r="E8" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="154"/>
+      <c r="F8" s="138"/>
       <c r="G8" s="10">
         <v>3</v>
       </c>
@@ -5739,45 +5739,45 @@
         <v>11</v>
       </c>
       <c r="I8" s="12"/>
-      <c r="J8" s="154" t="s">
+      <c r="J8" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="154"/>
-      <c r="L8" s="155"/>
-      <c r="M8" s="155"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="139"/>
+      <c r="M8" s="139"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A9" s="156" t="s">
+      <c r="A9" s="140" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="158" t="s">
+      <c r="B9" s="142" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="160" t="s">
+      <c r="C9" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="160"/>
-      <c r="E9" s="160"/>
-      <c r="F9" s="161" t="s">
+      <c r="D9" s="144"/>
+      <c r="E9" s="144"/>
+      <c r="F9" s="145" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="161" t="s">
+      <c r="G9" s="145" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="163"/>
-      <c r="I9" s="163"/>
-      <c r="J9" s="144" t="s">
+      <c r="H9" s="147"/>
+      <c r="I9" s="147"/>
+      <c r="J9" s="148" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="145"/>
-      <c r="L9" s="144" t="s">
+      <c r="K9" s="149"/>
+      <c r="L9" s="148" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="145"/>
+      <c r="M9" s="149"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="157"/>
-      <c r="B10" s="159"/>
+      <c r="A10" s="141"/>
+      <c r="B10" s="143"/>
       <c r="C10" s="13" t="s">
         <v>19</v>
       </c>
@@ -5787,14 +5787,14 @@
       <c r="E10" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="162"/>
-      <c r="G10" s="162"/>
-      <c r="H10" s="162"/>
-      <c r="I10" s="162"/>
-      <c r="J10" s="146"/>
-      <c r="K10" s="146"/>
-      <c r="L10" s="146"/>
-      <c r="M10" s="146"/>
+      <c r="F10" s="146"/>
+      <c r="G10" s="146"/>
+      <c r="H10" s="146"/>
+      <c r="I10" s="146"/>
+      <c r="J10" s="150"/>
+      <c r="K10" s="150"/>
+      <c r="L10" s="150"/>
+      <c r="M10" s="150"/>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="14">
@@ -5815,19 +5815,19 @@
       <c r="F11" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G11" s="147"/>
-      <c r="H11" s="148"/>
-      <c r="I11" s="149"/>
-      <c r="J11" s="150"/>
-      <c r="K11" s="151"/>
-      <c r="L11" s="147"/>
-      <c r="M11" s="149"/>
-      <c r="O11" s="136" t="s">
+      <c r="G11" s="155"/>
+      <c r="H11" s="156"/>
+      <c r="I11" s="157"/>
+      <c r="J11" s="158"/>
+      <c r="K11" s="159"/>
+      <c r="L11" s="155"/>
+      <c r="M11" s="157"/>
+      <c r="O11" s="168" t="s">
         <v>23</v>
       </c>
-      <c r="P11" s="137"/>
-      <c r="Q11" s="137"/>
-      <c r="R11" s="138"/>
+      <c r="P11" s="169"/>
+      <c r="Q11" s="169"/>
+      <c r="R11" s="170"/>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="14">
@@ -5848,21 +5848,21 @@
       <c r="F12" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G12" s="132"/>
-      <c r="H12" s="132"/>
-      <c r="I12" s="132"/>
-      <c r="J12" s="142"/>
-      <c r="K12" s="143"/>
-      <c r="L12" s="134"/>
-      <c r="M12" s="134"/>
+      <c r="G12" s="151"/>
+      <c r="H12" s="151"/>
+      <c r="I12" s="151"/>
+      <c r="J12" s="152"/>
+      <c r="K12" s="153"/>
+      <c r="L12" s="154"/>
+      <c r="M12" s="154"/>
       <c r="O12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="P12" s="131" t="s">
+      <c r="P12" s="166" t="s">
         <v>159</v>
       </c>
-      <c r="Q12" s="131"/>
-      <c r="R12" s="131"/>
+      <c r="Q12" s="166"/>
+      <c r="R12" s="166"/>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="14">
@@ -5883,21 +5883,21 @@
       <c r="F13" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G13" s="132"/>
-      <c r="H13" s="132"/>
-      <c r="I13" s="132"/>
-      <c r="J13" s="142"/>
-      <c r="K13" s="143"/>
-      <c r="L13" s="134"/>
-      <c r="M13" s="134"/>
+      <c r="G13" s="151"/>
+      <c r="H13" s="151"/>
+      <c r="I13" s="151"/>
+      <c r="J13" s="152"/>
+      <c r="K13" s="153"/>
+      <c r="L13" s="154"/>
+      <c r="M13" s="154"/>
       <c r="O13" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="P13" s="131" t="s">
+      <c r="P13" s="166" t="s">
         <v>165</v>
       </c>
-      <c r="Q13" s="131"/>
-      <c r="R13" s="131"/>
+      <c r="Q13" s="166"/>
+      <c r="R13" s="166"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="14">
@@ -5918,21 +5918,21 @@
       <c r="F14" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G14" s="132"/>
-      <c r="H14" s="132"/>
-      <c r="I14" s="132"/>
-      <c r="J14" s="142"/>
-      <c r="K14" s="143"/>
-      <c r="L14" s="134"/>
-      <c r="M14" s="134"/>
+      <c r="G14" s="151"/>
+      <c r="H14" s="151"/>
+      <c r="I14" s="151"/>
+      <c r="J14" s="152"/>
+      <c r="K14" s="153"/>
+      <c r="L14" s="154"/>
+      <c r="M14" s="154"/>
       <c r="O14" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="128" t="s">
+      <c r="P14" s="163" t="s">
         <v>160</v>
       </c>
-      <c r="Q14" s="129"/>
-      <c r="R14" s="130"/>
+      <c r="Q14" s="164"/>
+      <c r="R14" s="165"/>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="14">
@@ -5953,21 +5953,21 @@
       <c r="F15" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G15" s="132"/>
-      <c r="H15" s="132"/>
-      <c r="I15" s="132"/>
-      <c r="J15" s="142"/>
-      <c r="K15" s="143"/>
-      <c r="L15" s="134"/>
-      <c r="M15" s="134"/>
+      <c r="G15" s="151"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="151"/>
+      <c r="J15" s="152"/>
+      <c r="K15" s="153"/>
+      <c r="L15" s="154"/>
+      <c r="M15" s="154"/>
       <c r="O15" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="P15" s="128" t="s">
+      <c r="P15" s="163" t="s">
         <v>161</v>
       </c>
-      <c r="Q15" s="129"/>
-      <c r="R15" s="130"/>
+      <c r="Q15" s="164"/>
+      <c r="R15" s="165"/>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="14">
@@ -5988,21 +5988,21 @@
       <c r="F16" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G16" s="132"/>
-      <c r="H16" s="132"/>
-      <c r="I16" s="132"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="143"/>
-      <c r="L16" s="134"/>
-      <c r="M16" s="134"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="152"/>
+      <c r="K16" s="153"/>
+      <c r="L16" s="154"/>
+      <c r="M16" s="154"/>
       <c r="O16" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="P16" s="139" t="s">
+      <c r="P16" s="171" t="s">
         <v>163</v>
       </c>
-      <c r="Q16" s="140"/>
-      <c r="R16" s="141"/>
+      <c r="Q16" s="172"/>
+      <c r="R16" s="173"/>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="14">
@@ -6023,21 +6023,21 @@
       <c r="F17" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G17" s="132"/>
-      <c r="H17" s="132"/>
-      <c r="I17" s="132"/>
-      <c r="J17" s="142"/>
-      <c r="K17" s="143"/>
-      <c r="L17" s="134"/>
-      <c r="M17" s="134"/>
+      <c r="G17" s="151"/>
+      <c r="H17" s="151"/>
+      <c r="I17" s="151"/>
+      <c r="J17" s="152"/>
+      <c r="K17" s="153"/>
+      <c r="L17" s="154"/>
+      <c r="M17" s="154"/>
       <c r="O17" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="P17" s="128" t="s">
+      <c r="P17" s="163" t="s">
         <v>162</v>
       </c>
-      <c r="Q17" s="129"/>
-      <c r="R17" s="130"/>
+      <c r="Q17" s="164"/>
+      <c r="R17" s="165"/>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="14">
@@ -6058,13 +6058,13 @@
       <c r="F18" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G18" s="132"/>
-      <c r="H18" s="132"/>
-      <c r="I18" s="132"/>
-      <c r="J18" s="142"/>
-      <c r="K18" s="143"/>
-      <c r="L18" s="134"/>
-      <c r="M18" s="134"/>
+      <c r="G18" s="151"/>
+      <c r="H18" s="151"/>
+      <c r="I18" s="151"/>
+      <c r="J18" s="152"/>
+      <c r="K18" s="153"/>
+      <c r="L18" s="154"/>
+      <c r="M18" s="154"/>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="14">
@@ -6085,13 +6085,13 @@
       <c r="F19" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G19" s="132"/>
-      <c r="H19" s="132"/>
-      <c r="I19" s="132"/>
-      <c r="J19" s="142"/>
-      <c r="K19" s="143"/>
-      <c r="L19" s="134"/>
-      <c r="M19" s="134"/>
+      <c r="G19" s="151"/>
+      <c r="H19" s="151"/>
+      <c r="I19" s="151"/>
+      <c r="J19" s="152"/>
+      <c r="K19" s="153"/>
+      <c r="L19" s="154"/>
+      <c r="M19" s="154"/>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="14">
@@ -6112,13 +6112,13 @@
       <c r="F20" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G20" s="132"/>
-      <c r="H20" s="132"/>
-      <c r="I20" s="132"/>
-      <c r="J20" s="142"/>
-      <c r="K20" s="143"/>
-      <c r="L20" s="134"/>
-      <c r="M20" s="134"/>
+      <c r="G20" s="151"/>
+      <c r="H20" s="151"/>
+      <c r="I20" s="151"/>
+      <c r="J20" s="152"/>
+      <c r="K20" s="153"/>
+      <c r="L20" s="154"/>
+      <c r="M20" s="154"/>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="14">
@@ -6139,13 +6139,13 @@
       <c r="F21" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G21" s="132"/>
-      <c r="H21" s="132"/>
-      <c r="I21" s="132"/>
-      <c r="J21" s="142"/>
-      <c r="K21" s="143"/>
-      <c r="L21" s="134"/>
-      <c r="M21" s="134"/>
+      <c r="G21" s="151"/>
+      <c r="H21" s="151"/>
+      <c r="I21" s="151"/>
+      <c r="J21" s="152"/>
+      <c r="K21" s="153"/>
+      <c r="L21" s="154"/>
+      <c r="M21" s="154"/>
       <c r="P21" s="99" t="s">
         <v>143</v>
       </c>
@@ -6169,13 +6169,13 @@
       <c r="F22" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G22" s="132"/>
-      <c r="H22" s="132"/>
-      <c r="I22" s="132"/>
-      <c r="J22" s="142"/>
-      <c r="K22" s="143"/>
-      <c r="L22" s="134"/>
-      <c r="M22" s="134"/>
+      <c r="G22" s="151"/>
+      <c r="H22" s="151"/>
+      <c r="I22" s="151"/>
+      <c r="J22" s="152"/>
+      <c r="K22" s="153"/>
+      <c r="L22" s="154"/>
+      <c r="M22" s="154"/>
       <c r="P22" s="100">
         <v>0</v>
       </c>
@@ -6202,13 +6202,13 @@
       <c r="F23" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G23" s="132"/>
-      <c r="H23" s="132"/>
-      <c r="I23" s="132"/>
-      <c r="J23" s="142"/>
-      <c r="K23" s="143"/>
-      <c r="L23" s="134"/>
-      <c r="M23" s="134"/>
+      <c r="G23" s="151"/>
+      <c r="H23" s="151"/>
+      <c r="I23" s="151"/>
+      <c r="J23" s="152"/>
+      <c r="K23" s="153"/>
+      <c r="L23" s="154"/>
+      <c r="M23" s="154"/>
       <c r="P23" s="101">
         <v>70</v>
       </c>
@@ -6235,13 +6235,13 @@
       <c r="F24" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G24" s="132"/>
-      <c r="H24" s="132"/>
-      <c r="I24" s="132"/>
-      <c r="J24" s="142"/>
-      <c r="K24" s="143"/>
-      <c r="L24" s="134"/>
-      <c r="M24" s="134"/>
+      <c r="G24" s="151"/>
+      <c r="H24" s="151"/>
+      <c r="I24" s="151"/>
+      <c r="J24" s="152"/>
+      <c r="K24" s="153"/>
+      <c r="L24" s="154"/>
+      <c r="M24" s="154"/>
       <c r="P24" s="101">
         <v>73.34</v>
       </c>
@@ -6268,13 +6268,13 @@
       <c r="F25" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G25" s="132"/>
-      <c r="H25" s="132"/>
-      <c r="I25" s="132"/>
-      <c r="J25" s="142"/>
-      <c r="K25" s="143"/>
-      <c r="L25" s="134"/>
-      <c r="M25" s="134"/>
+      <c r="G25" s="151"/>
+      <c r="H25" s="151"/>
+      <c r="I25" s="151"/>
+      <c r="J25" s="152"/>
+      <c r="K25" s="153"/>
+      <c r="L25" s="154"/>
+      <c r="M25" s="154"/>
       <c r="P25" s="101">
         <v>76.680000000000007</v>
       </c>
@@ -6301,13 +6301,13 @@
       <c r="F26" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G26" s="132"/>
-      <c r="H26" s="132"/>
-      <c r="I26" s="132"/>
-      <c r="J26" s="142"/>
-      <c r="K26" s="143"/>
-      <c r="L26" s="134"/>
-      <c r="M26" s="134"/>
+      <c r="G26" s="151"/>
+      <c r="H26" s="151"/>
+      <c r="I26" s="151"/>
+      <c r="J26" s="152"/>
+      <c r="K26" s="153"/>
+      <c r="L26" s="154"/>
+      <c r="M26" s="154"/>
       <c r="P26" s="101">
         <v>80.02</v>
       </c>
@@ -6334,13 +6334,13 @@
       <c r="F27" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G27" s="132"/>
-      <c r="H27" s="132"/>
-      <c r="I27" s="132"/>
-      <c r="J27" s="142"/>
-      <c r="K27" s="143"/>
-      <c r="L27" s="134"/>
-      <c r="M27" s="134"/>
+      <c r="G27" s="151"/>
+      <c r="H27" s="151"/>
+      <c r="I27" s="151"/>
+      <c r="J27" s="152"/>
+      <c r="K27" s="153"/>
+      <c r="L27" s="154"/>
+      <c r="M27" s="154"/>
       <c r="P27" s="101">
         <v>83.36</v>
       </c>
@@ -6367,13 +6367,13 @@
       <c r="F28" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G28" s="132"/>
-      <c r="H28" s="132"/>
-      <c r="I28" s="132"/>
-      <c r="J28" s="142"/>
-      <c r="K28" s="143"/>
-      <c r="L28" s="134"/>
-      <c r="M28" s="134"/>
+      <c r="G28" s="151"/>
+      <c r="H28" s="151"/>
+      <c r="I28" s="151"/>
+      <c r="J28" s="152"/>
+      <c r="K28" s="153"/>
+      <c r="L28" s="154"/>
+      <c r="M28" s="154"/>
       <c r="P28" s="101">
         <v>86.7</v>
       </c>
@@ -6400,13 +6400,13 @@
       <c r="F29" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G29" s="132"/>
-      <c r="H29" s="132"/>
-      <c r="I29" s="132"/>
-      <c r="J29" s="142"/>
-      <c r="K29" s="143"/>
-      <c r="L29" s="134"/>
-      <c r="M29" s="134"/>
+      <c r="G29" s="151"/>
+      <c r="H29" s="151"/>
+      <c r="I29" s="151"/>
+      <c r="J29" s="152"/>
+      <c r="K29" s="153"/>
+      <c r="L29" s="154"/>
+      <c r="M29" s="154"/>
       <c r="P29" s="101">
         <v>90.04</v>
       </c>
@@ -6433,13 +6433,13 @@
       <c r="F30" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G30" s="132"/>
-      <c r="H30" s="132"/>
-      <c r="I30" s="132"/>
-      <c r="J30" s="142"/>
-      <c r="K30" s="143"/>
-      <c r="L30" s="134"/>
-      <c r="M30" s="134"/>
+      <c r="G30" s="151"/>
+      <c r="H30" s="151"/>
+      <c r="I30" s="151"/>
+      <c r="J30" s="152"/>
+      <c r="K30" s="153"/>
+      <c r="L30" s="154"/>
+      <c r="M30" s="154"/>
       <c r="P30" s="101">
         <v>93.38</v>
       </c>
@@ -6466,13 +6466,13 @@
       <c r="F31" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G31" s="132"/>
-      <c r="H31" s="132"/>
-      <c r="I31" s="132"/>
-      <c r="J31" s="142"/>
-      <c r="K31" s="143"/>
-      <c r="L31" s="134"/>
-      <c r="M31" s="134"/>
+      <c r="G31" s="151"/>
+      <c r="H31" s="151"/>
+      <c r="I31" s="151"/>
+      <c r="J31" s="152"/>
+      <c r="K31" s="153"/>
+      <c r="L31" s="154"/>
+      <c r="M31" s="154"/>
       <c r="P31" s="100"/>
       <c r="Q31" s="100"/>
     </row>
@@ -6495,13 +6495,13 @@
       <c r="F32" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G32" s="132"/>
-      <c r="H32" s="132"/>
-      <c r="I32" s="132"/>
-      <c r="J32" s="142"/>
-      <c r="K32" s="143"/>
-      <c r="L32" s="134"/>
-      <c r="M32" s="134"/>
+      <c r="G32" s="151"/>
+      <c r="H32" s="151"/>
+      <c r="I32" s="151"/>
+      <c r="J32" s="152"/>
+      <c r="K32" s="153"/>
+      <c r="L32" s="154"/>
+      <c r="M32" s="154"/>
       <c r="P32" s="100">
         <v>96.72</v>
       </c>
@@ -6528,13 +6528,13 @@
       <c r="F33" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G33" s="132"/>
-      <c r="H33" s="132"/>
-      <c r="I33" s="132"/>
-      <c r="J33" s="142"/>
-      <c r="K33" s="143"/>
-      <c r="L33" s="134"/>
-      <c r="M33" s="134"/>
+      <c r="G33" s="151"/>
+      <c r="H33" s="151"/>
+      <c r="I33" s="151"/>
+      <c r="J33" s="152"/>
+      <c r="K33" s="153"/>
+      <c r="L33" s="154"/>
+      <c r="M33" s="154"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="14">
@@ -6555,13 +6555,13 @@
       <c r="F34" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G34" s="132"/>
-      <c r="H34" s="132"/>
-      <c r="I34" s="132"/>
-      <c r="J34" s="142"/>
-      <c r="K34" s="143"/>
-      <c r="L34" s="134"/>
-      <c r="M34" s="134"/>
+      <c r="G34" s="151"/>
+      <c r="H34" s="151"/>
+      <c r="I34" s="151"/>
+      <c r="J34" s="152"/>
+      <c r="K34" s="153"/>
+      <c r="L34" s="154"/>
+      <c r="M34" s="154"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="14">
@@ -6582,13 +6582,13 @@
       <c r="F35" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G35" s="132"/>
-      <c r="H35" s="132"/>
-      <c r="I35" s="132"/>
-      <c r="J35" s="142"/>
-      <c r="K35" s="143"/>
-      <c r="L35" s="134"/>
-      <c r="M35" s="134"/>
+      <c r="G35" s="151"/>
+      <c r="H35" s="151"/>
+      <c r="I35" s="151"/>
+      <c r="J35" s="152"/>
+      <c r="K35" s="153"/>
+      <c r="L35" s="154"/>
+      <c r="M35" s="154"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="14">
@@ -6609,13 +6609,13 @@
       <c r="F36" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G36" s="132"/>
-      <c r="H36" s="132"/>
-      <c r="I36" s="132"/>
-      <c r="J36" s="142"/>
-      <c r="K36" s="143"/>
-      <c r="L36" s="134"/>
-      <c r="M36" s="134"/>
+      <c r="G36" s="151"/>
+      <c r="H36" s="151"/>
+      <c r="I36" s="151"/>
+      <c r="J36" s="152"/>
+      <c r="K36" s="153"/>
+      <c r="L36" s="154"/>
+      <c r="M36" s="154"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="14">
@@ -6636,13 +6636,13 @@
       <c r="F37" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G37" s="132"/>
-      <c r="H37" s="132"/>
-      <c r="I37" s="132"/>
-      <c r="J37" s="133"/>
-      <c r="K37" s="133"/>
-      <c r="L37" s="134"/>
-      <c r="M37" s="134"/>
+      <c r="G37" s="151"/>
+      <c r="H37" s="151"/>
+      <c r="I37" s="151"/>
+      <c r="J37" s="160"/>
+      <c r="K37" s="160"/>
+      <c r="L37" s="154"/>
+      <c r="M37" s="154"/>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="14">
@@ -6663,13 +6663,13 @@
       <c r="F38" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G38" s="132"/>
-      <c r="H38" s="132"/>
-      <c r="I38" s="132"/>
-      <c r="J38" s="133"/>
-      <c r="K38" s="133"/>
-      <c r="L38" s="134"/>
-      <c r="M38" s="134"/>
+      <c r="G38" s="151"/>
+      <c r="H38" s="151"/>
+      <c r="I38" s="151"/>
+      <c r="J38" s="160"/>
+      <c r="K38" s="160"/>
+      <c r="L38" s="154"/>
+      <c r="M38" s="154"/>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="14">
@@ -6690,13 +6690,13 @@
       <c r="F39" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G39" s="132"/>
-      <c r="H39" s="132"/>
-      <c r="I39" s="132"/>
-      <c r="J39" s="133"/>
-      <c r="K39" s="133"/>
-      <c r="L39" s="134"/>
-      <c r="M39" s="134"/>
+      <c r="G39" s="151"/>
+      <c r="H39" s="151"/>
+      <c r="I39" s="151"/>
+      <c r="J39" s="160"/>
+      <c r="K39" s="160"/>
+      <c r="L39" s="154"/>
+      <c r="M39" s="154"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="14">
@@ -6717,13 +6717,13 @@
       <c r="F40" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G40" s="132"/>
-      <c r="H40" s="132"/>
-      <c r="I40" s="132"/>
-      <c r="J40" s="133"/>
-      <c r="K40" s="133"/>
-      <c r="L40" s="134"/>
-      <c r="M40" s="134"/>
+      <c r="G40" s="151"/>
+      <c r="H40" s="151"/>
+      <c r="I40" s="151"/>
+      <c r="J40" s="160"/>
+      <c r="K40" s="160"/>
+      <c r="L40" s="154"/>
+      <c r="M40" s="154"/>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="14">
@@ -6744,13 +6744,13 @@
       <c r="F41" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G41" s="132"/>
-      <c r="H41" s="132"/>
-      <c r="I41" s="132"/>
-      <c r="J41" s="133"/>
-      <c r="K41" s="133"/>
-      <c r="L41" s="134"/>
-      <c r="M41" s="134"/>
+      <c r="G41" s="151"/>
+      <c r="H41" s="151"/>
+      <c r="I41" s="151"/>
+      <c r="J41" s="160"/>
+      <c r="K41" s="160"/>
+      <c r="L41" s="154"/>
+      <c r="M41" s="154"/>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="14">
@@ -6771,13 +6771,13 @@
       <c r="F42" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G42" s="132"/>
-      <c r="H42" s="132"/>
-      <c r="I42" s="132"/>
-      <c r="J42" s="133"/>
-      <c r="K42" s="133"/>
-      <c r="L42" s="134"/>
-      <c r="M42" s="134"/>
+      <c r="G42" s="151"/>
+      <c r="H42" s="151"/>
+      <c r="I42" s="151"/>
+      <c r="J42" s="160"/>
+      <c r="K42" s="160"/>
+      <c r="L42" s="154"/>
+      <c r="M42" s="154"/>
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="14">
@@ -6798,13 +6798,13 @@
       <c r="F43" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G43" s="132"/>
-      <c r="H43" s="132"/>
-      <c r="I43" s="132"/>
-      <c r="J43" s="133"/>
-      <c r="K43" s="133"/>
-      <c r="L43" s="134"/>
-      <c r="M43" s="134"/>
+      <c r="G43" s="151"/>
+      <c r="H43" s="151"/>
+      <c r="I43" s="151"/>
+      <c r="J43" s="160"/>
+      <c r="K43" s="160"/>
+      <c r="L43" s="154"/>
+      <c r="M43" s="154"/>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="14">
@@ -6825,13 +6825,13 @@
       <c r="F44" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G44" s="132"/>
-      <c r="H44" s="132"/>
-      <c r="I44" s="132"/>
-      <c r="J44" s="133"/>
-      <c r="K44" s="133"/>
-      <c r="L44" s="134"/>
-      <c r="M44" s="134"/>
+      <c r="G44" s="151"/>
+      <c r="H44" s="151"/>
+      <c r="I44" s="151"/>
+      <c r="J44" s="160"/>
+      <c r="K44" s="160"/>
+      <c r="L44" s="154"/>
+      <c r="M44" s="154"/>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="14">
@@ -6852,13 +6852,13 @@
       <c r="F45" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G45" s="132"/>
-      <c r="H45" s="132"/>
-      <c r="I45" s="132"/>
-      <c r="J45" s="133"/>
-      <c r="K45" s="133"/>
-      <c r="L45" s="134"/>
-      <c r="M45" s="134"/>
+      <c r="G45" s="151"/>
+      <c r="H45" s="151"/>
+      <c r="I45" s="151"/>
+      <c r="J45" s="160"/>
+      <c r="K45" s="160"/>
+      <c r="L45" s="154"/>
+      <c r="M45" s="154"/>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="14">
@@ -6879,13 +6879,13 @@
       <c r="F46" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G46" s="132"/>
-      <c r="H46" s="132"/>
-      <c r="I46" s="132"/>
-      <c r="J46" s="133"/>
-      <c r="K46" s="133"/>
-      <c r="L46" s="134"/>
-      <c r="M46" s="134"/>
+      <c r="G46" s="151"/>
+      <c r="H46" s="151"/>
+      <c r="I46" s="151"/>
+      <c r="J46" s="160"/>
+      <c r="K46" s="160"/>
+      <c r="L46" s="154"/>
+      <c r="M46" s="154"/>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="14">
@@ -6906,13 +6906,13 @@
       <c r="F47" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G47" s="132"/>
-      <c r="H47" s="132"/>
-      <c r="I47" s="132"/>
-      <c r="J47" s="133"/>
-      <c r="K47" s="133"/>
-      <c r="L47" s="134"/>
-      <c r="M47" s="134"/>
+      <c r="G47" s="151"/>
+      <c r="H47" s="151"/>
+      <c r="I47" s="151"/>
+      <c r="J47" s="160"/>
+      <c r="K47" s="160"/>
+      <c r="L47" s="154"/>
+      <c r="M47" s="154"/>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="14">
@@ -6933,13 +6933,13 @@
       <c r="F48" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G48" s="132"/>
-      <c r="H48" s="132"/>
-      <c r="I48" s="132"/>
-      <c r="J48" s="133"/>
-      <c r="K48" s="133"/>
-      <c r="L48" s="134"/>
-      <c r="M48" s="134"/>
+      <c r="G48" s="151"/>
+      <c r="H48" s="151"/>
+      <c r="I48" s="151"/>
+      <c r="J48" s="160"/>
+      <c r="K48" s="160"/>
+      <c r="L48" s="154"/>
+      <c r="M48" s="154"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="14">
@@ -6960,13 +6960,13 @@
       <c r="F49" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G49" s="132"/>
-      <c r="H49" s="132"/>
-      <c r="I49" s="132"/>
-      <c r="J49" s="133"/>
-      <c r="K49" s="133"/>
-      <c r="L49" s="134"/>
-      <c r="M49" s="134"/>
+      <c r="G49" s="151"/>
+      <c r="H49" s="151"/>
+      <c r="I49" s="151"/>
+      <c r="J49" s="160"/>
+      <c r="K49" s="160"/>
+      <c r="L49" s="154"/>
+      <c r="M49" s="154"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="14">
@@ -6987,13 +6987,13 @@
       <c r="F50" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G50" s="132"/>
-      <c r="H50" s="132"/>
-      <c r="I50" s="132"/>
-      <c r="J50" s="133"/>
-      <c r="K50" s="133"/>
-      <c r="L50" s="134"/>
-      <c r="M50" s="134"/>
+      <c r="G50" s="151"/>
+      <c r="H50" s="151"/>
+      <c r="I50" s="151"/>
+      <c r="J50" s="160"/>
+      <c r="K50" s="160"/>
+      <c r="L50" s="154"/>
+      <c r="M50" s="154"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="14">
@@ -7014,13 +7014,13 @@
       <c r="F51" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G51" s="132"/>
-      <c r="H51" s="132"/>
-      <c r="I51" s="132"/>
-      <c r="J51" s="133"/>
-      <c r="K51" s="133"/>
-      <c r="L51" s="134"/>
-      <c r="M51" s="134"/>
+      <c r="G51" s="151"/>
+      <c r="H51" s="151"/>
+      <c r="I51" s="151"/>
+      <c r="J51" s="160"/>
+      <c r="K51" s="160"/>
+      <c r="L51" s="154"/>
+      <c r="M51" s="154"/>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="14">
@@ -7041,13 +7041,13 @@
       <c r="F52" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G52" s="132"/>
-      <c r="H52" s="132"/>
-      <c r="I52" s="132"/>
-      <c r="J52" s="133"/>
-      <c r="K52" s="133"/>
-      <c r="L52" s="134"/>
-      <c r="M52" s="134"/>
+      <c r="G52" s="151"/>
+      <c r="H52" s="151"/>
+      <c r="I52" s="151"/>
+      <c r="J52" s="160"/>
+      <c r="K52" s="160"/>
+      <c r="L52" s="154"/>
+      <c r="M52" s="154"/>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="14">
@@ -7068,13 +7068,13 @@
       <c r="F53" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G53" s="132"/>
-      <c r="H53" s="132"/>
-      <c r="I53" s="132"/>
-      <c r="J53" s="133"/>
-      <c r="K53" s="133"/>
-      <c r="L53" s="134"/>
-      <c r="M53" s="134"/>
+      <c r="G53" s="151"/>
+      <c r="H53" s="151"/>
+      <c r="I53" s="151"/>
+      <c r="J53" s="160"/>
+      <c r="K53" s="160"/>
+      <c r="L53" s="154"/>
+      <c r="M53" s="154"/>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="14">
@@ -7095,13 +7095,13 @@
       <c r="F54" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G54" s="132"/>
-      <c r="H54" s="132"/>
-      <c r="I54" s="132"/>
-      <c r="J54" s="133"/>
-      <c r="K54" s="133"/>
-      <c r="L54" s="134"/>
-      <c r="M54" s="134"/>
+      <c r="G54" s="151"/>
+      <c r="H54" s="151"/>
+      <c r="I54" s="151"/>
+      <c r="J54" s="160"/>
+      <c r="K54" s="160"/>
+      <c r="L54" s="154"/>
+      <c r="M54" s="154"/>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="14">
@@ -7122,13 +7122,13 @@
       <c r="F55" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G55" s="132"/>
-      <c r="H55" s="132"/>
-      <c r="I55" s="132"/>
-      <c r="J55" s="133"/>
-      <c r="K55" s="133"/>
-      <c r="L55" s="134"/>
-      <c r="M55" s="134"/>
+      <c r="G55" s="151"/>
+      <c r="H55" s="151"/>
+      <c r="I55" s="151"/>
+      <c r="J55" s="160"/>
+      <c r="K55" s="160"/>
+      <c r="L55" s="154"/>
+      <c r="M55" s="154"/>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="14">
@@ -7149,13 +7149,13 @@
       <c r="F56" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G56" s="132"/>
-      <c r="H56" s="132"/>
-      <c r="I56" s="132"/>
-      <c r="J56" s="133"/>
-      <c r="K56" s="133"/>
-      <c r="L56" s="134"/>
-      <c r="M56" s="134"/>
+      <c r="G56" s="151"/>
+      <c r="H56" s="151"/>
+      <c r="I56" s="151"/>
+      <c r="J56" s="160"/>
+      <c r="K56" s="160"/>
+      <c r="L56" s="154"/>
+      <c r="M56" s="154"/>
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="14">
@@ -7176,13 +7176,13 @@
       <c r="F57" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G57" s="132"/>
-      <c r="H57" s="132"/>
-      <c r="I57" s="132"/>
-      <c r="J57" s="133"/>
-      <c r="K57" s="133"/>
-      <c r="L57" s="134"/>
-      <c r="M57" s="134"/>
+      <c r="G57" s="151"/>
+      <c r="H57" s="151"/>
+      <c r="I57" s="151"/>
+      <c r="J57" s="160"/>
+      <c r="K57" s="160"/>
+      <c r="L57" s="154"/>
+      <c r="M57" s="154"/>
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="14">
@@ -7203,13 +7203,13 @@
       <c r="F58" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G58" s="132"/>
-      <c r="H58" s="132"/>
-      <c r="I58" s="132"/>
-      <c r="J58" s="133"/>
-      <c r="K58" s="133"/>
-      <c r="L58" s="134"/>
-      <c r="M58" s="134"/>
+      <c r="G58" s="151"/>
+      <c r="H58" s="151"/>
+      <c r="I58" s="151"/>
+      <c r="J58" s="160"/>
+      <c r="K58" s="160"/>
+      <c r="L58" s="154"/>
+      <c r="M58" s="154"/>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="14">
@@ -7230,13 +7230,13 @@
       <c r="F59" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G59" s="132"/>
-      <c r="H59" s="132"/>
-      <c r="I59" s="132"/>
-      <c r="J59" s="133"/>
-      <c r="K59" s="133"/>
-      <c r="L59" s="134"/>
-      <c r="M59" s="134"/>
+      <c r="G59" s="151"/>
+      <c r="H59" s="151"/>
+      <c r="I59" s="151"/>
+      <c r="J59" s="160"/>
+      <c r="K59" s="160"/>
+      <c r="L59" s="154"/>
+      <c r="M59" s="154"/>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="14">
@@ -7257,13 +7257,13 @@
       <c r="F60" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G60" s="132"/>
-      <c r="H60" s="132"/>
-      <c r="I60" s="132"/>
-      <c r="J60" s="133"/>
-      <c r="K60" s="133"/>
-      <c r="L60" s="134"/>
-      <c r="M60" s="134"/>
+      <c r="G60" s="151"/>
+      <c r="H60" s="151"/>
+      <c r="I60" s="151"/>
+      <c r="J60" s="160"/>
+      <c r="K60" s="160"/>
+      <c r="L60" s="154"/>
+      <c r="M60" s="154"/>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="14">
@@ -7274,13 +7274,13 @@
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
       <c r="F61" s="16"/>
-      <c r="G61" s="132"/>
-      <c r="H61" s="132"/>
-      <c r="I61" s="132"/>
-      <c r="J61" s="133"/>
-      <c r="K61" s="133"/>
-      <c r="L61" s="134"/>
-      <c r="M61" s="134"/>
+      <c r="G61" s="151"/>
+      <c r="H61" s="151"/>
+      <c r="I61" s="151"/>
+      <c r="J61" s="160"/>
+      <c r="K61" s="160"/>
+      <c r="L61" s="154"/>
+      <c r="M61" s="154"/>
     </row>
     <row r="62" spans="1:13">
       <c r="A62" s="14">
@@ -7291,13 +7291,13 @@
       <c r="D62" s="15"/>
       <c r="E62" s="15"/>
       <c r="F62" s="16"/>
-      <c r="G62" s="132"/>
-      <c r="H62" s="132"/>
-      <c r="I62" s="132"/>
-      <c r="J62" s="133"/>
-      <c r="K62" s="133"/>
-      <c r="L62" s="134"/>
-      <c r="M62" s="134"/>
+      <c r="G62" s="151"/>
+      <c r="H62" s="151"/>
+      <c r="I62" s="151"/>
+      <c r="J62" s="160"/>
+      <c r="K62" s="160"/>
+      <c r="L62" s="154"/>
+      <c r="M62" s="154"/>
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="14">
@@ -7308,13 +7308,13 @@
       <c r="D63" s="15"/>
       <c r="E63" s="15"/>
       <c r="F63" s="16"/>
-      <c r="G63" s="132"/>
-      <c r="H63" s="132"/>
-      <c r="I63" s="132"/>
-      <c r="J63" s="133"/>
-      <c r="K63" s="133"/>
-      <c r="L63" s="134"/>
-      <c r="M63" s="134"/>
+      <c r="G63" s="151"/>
+      <c r="H63" s="151"/>
+      <c r="I63" s="151"/>
+      <c r="J63" s="160"/>
+      <c r="K63" s="160"/>
+      <c r="L63" s="154"/>
+      <c r="M63" s="154"/>
     </row>
     <row r="64" spans="1:13">
       <c r="A64" s="14">
@@ -7325,13 +7325,13 @@
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
       <c r="F64" s="16"/>
-      <c r="G64" s="132"/>
-      <c r="H64" s="132"/>
-      <c r="I64" s="132"/>
-      <c r="J64" s="133"/>
-      <c r="K64" s="133"/>
-      <c r="L64" s="134"/>
-      <c r="M64" s="134"/>
+      <c r="G64" s="151"/>
+      <c r="H64" s="151"/>
+      <c r="I64" s="151"/>
+      <c r="J64" s="160"/>
+      <c r="K64" s="160"/>
+      <c r="L64" s="154"/>
+      <c r="M64" s="154"/>
     </row>
     <row r="65" spans="1:13">
       <c r="A65" s="14">
@@ -7342,13 +7342,13 @@
       <c r="D65" s="15"/>
       <c r="E65" s="15"/>
       <c r="F65" s="16"/>
-      <c r="G65" s="132"/>
-      <c r="H65" s="132"/>
-      <c r="I65" s="132"/>
-      <c r="J65" s="133"/>
-      <c r="K65" s="133"/>
-      <c r="L65" s="134"/>
-      <c r="M65" s="134"/>
+      <c r="G65" s="151"/>
+      <c r="H65" s="151"/>
+      <c r="I65" s="151"/>
+      <c r="J65" s="160"/>
+      <c r="K65" s="160"/>
+      <c r="L65" s="154"/>
+      <c r="M65" s="154"/>
     </row>
     <row r="66" spans="1:13">
       <c r="A66" s="14">
@@ -7359,13 +7359,13 @@
       <c r="D66" s="15"/>
       <c r="E66" s="15"/>
       <c r="F66" s="16"/>
-      <c r="G66" s="132"/>
-      <c r="H66" s="132"/>
-      <c r="I66" s="132"/>
-      <c r="J66" s="133"/>
-      <c r="K66" s="133"/>
-      <c r="L66" s="134"/>
-      <c r="M66" s="134"/>
+      <c r="G66" s="151"/>
+      <c r="H66" s="151"/>
+      <c r="I66" s="151"/>
+      <c r="J66" s="160"/>
+      <c r="K66" s="160"/>
+      <c r="L66" s="154"/>
+      <c r="M66" s="154"/>
     </row>
     <row r="67" spans="1:13">
       <c r="A67" s="14">
@@ -7376,13 +7376,13 @@
       <c r="D67" s="15"/>
       <c r="E67" s="89"/>
       <c r="F67" s="16"/>
-      <c r="G67" s="132"/>
-      <c r="H67" s="132"/>
-      <c r="I67" s="132"/>
-      <c r="J67" s="133"/>
-      <c r="K67" s="133"/>
-      <c r="L67" s="134"/>
-      <c r="M67" s="134"/>
+      <c r="G67" s="151"/>
+      <c r="H67" s="151"/>
+      <c r="I67" s="151"/>
+      <c r="J67" s="160"/>
+      <c r="K67" s="160"/>
+      <c r="L67" s="154"/>
+      <c r="M67" s="154"/>
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="14">
@@ -7393,13 +7393,13 @@
       <c r="D68" s="15"/>
       <c r="E68" s="15"/>
       <c r="F68" s="16"/>
-      <c r="G68" s="132"/>
-      <c r="H68" s="132"/>
-      <c r="I68" s="132"/>
-      <c r="J68" s="133"/>
-      <c r="K68" s="133"/>
-      <c r="L68" s="134"/>
-      <c r="M68" s="134"/>
+      <c r="G68" s="151"/>
+      <c r="H68" s="151"/>
+      <c r="I68" s="151"/>
+      <c r="J68" s="160"/>
+      <c r="K68" s="160"/>
+      <c r="L68" s="154"/>
+      <c r="M68" s="154"/>
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="14">
@@ -7410,13 +7410,13 @@
       <c r="D69" s="15"/>
       <c r="E69" s="15"/>
       <c r="F69" s="16"/>
-      <c r="G69" s="132"/>
-      <c r="H69" s="132"/>
-      <c r="I69" s="132"/>
-      <c r="J69" s="133"/>
-      <c r="K69" s="133"/>
-      <c r="L69" s="134"/>
-      <c r="M69" s="134"/>
+      <c r="G69" s="151"/>
+      <c r="H69" s="151"/>
+      <c r="I69" s="151"/>
+      <c r="J69" s="160"/>
+      <c r="K69" s="160"/>
+      <c r="L69" s="154"/>
+      <c r="M69" s="154"/>
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="14">
@@ -7427,13 +7427,13 @@
       <c r="D70" s="15"/>
       <c r="E70" s="15"/>
       <c r="F70" s="16"/>
-      <c r="G70" s="132"/>
-      <c r="H70" s="132"/>
-      <c r="I70" s="132"/>
-      <c r="J70" s="133"/>
-      <c r="K70" s="133"/>
-      <c r="L70" s="134"/>
-      <c r="M70" s="134"/>
+      <c r="G70" s="151"/>
+      <c r="H70" s="151"/>
+      <c r="I70" s="151"/>
+      <c r="J70" s="160"/>
+      <c r="K70" s="160"/>
+      <c r="L70" s="154"/>
+      <c r="M70" s="154"/>
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="14">
@@ -7444,13 +7444,13 @@
       <c r="D71" s="89"/>
       <c r="E71" s="89"/>
       <c r="F71" s="16"/>
-      <c r="G71" s="132"/>
-      <c r="H71" s="132"/>
-      <c r="I71" s="132"/>
-      <c r="J71" s="133"/>
-      <c r="K71" s="133"/>
-      <c r="L71" s="134"/>
-      <c r="M71" s="134"/>
+      <c r="G71" s="151"/>
+      <c r="H71" s="151"/>
+      <c r="I71" s="151"/>
+      <c r="J71" s="160"/>
+      <c r="K71" s="160"/>
+      <c r="L71" s="154"/>
+      <c r="M71" s="154"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -7458,195 +7458,6 @@
     <sortCondition ref="C11:C33"/>
   </sortState>
   <mergeCells count="213">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:I10"/>
-    <mergeCell ref="J9:K10"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="L9:M10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="L49:M49"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="L50:M50"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="G53:I53"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="L53:M53"/>
-    <mergeCell ref="G54:I54"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="L54:M54"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="L51:M51"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="L52:M52"/>
-    <mergeCell ref="G57:I57"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="L57:M57"/>
-    <mergeCell ref="G58:I58"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="L58:M58"/>
-    <mergeCell ref="G55:I55"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="L55:M55"/>
-    <mergeCell ref="G56:I56"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="L56:M56"/>
-    <mergeCell ref="G61:I61"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="L61:M61"/>
-    <mergeCell ref="G62:I62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="L62:M62"/>
-    <mergeCell ref="G59:I59"/>
-    <mergeCell ref="J59:K59"/>
-    <mergeCell ref="L59:M59"/>
-    <mergeCell ref="G60:I60"/>
-    <mergeCell ref="J60:K60"/>
-    <mergeCell ref="L60:M60"/>
-    <mergeCell ref="L68:M68"/>
-    <mergeCell ref="G65:I65"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="L65:M65"/>
-    <mergeCell ref="G66:I66"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="L66:M66"/>
-    <mergeCell ref="G63:I63"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="L63:M63"/>
-    <mergeCell ref="G64:I64"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="L64:M64"/>
     <mergeCell ref="A5:M5"/>
     <mergeCell ref="A4:M4"/>
     <mergeCell ref="P15:R15"/>
@@ -7671,6 +7482,195 @@
     <mergeCell ref="L67:M67"/>
     <mergeCell ref="G68:I68"/>
     <mergeCell ref="J68:K68"/>
+    <mergeCell ref="L68:M68"/>
+    <mergeCell ref="G65:I65"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="L65:M65"/>
+    <mergeCell ref="G66:I66"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="L66:M66"/>
+    <mergeCell ref="G63:I63"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="L63:M63"/>
+    <mergeCell ref="G64:I64"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="L64:M64"/>
+    <mergeCell ref="G61:I61"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="L61:M61"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="L62:M62"/>
+    <mergeCell ref="G59:I59"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="L59:M59"/>
+    <mergeCell ref="G60:I60"/>
+    <mergeCell ref="J60:K60"/>
+    <mergeCell ref="L60:M60"/>
+    <mergeCell ref="G57:I57"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="L57:M57"/>
+    <mergeCell ref="G58:I58"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="L58:M58"/>
+    <mergeCell ref="G55:I55"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="L55:M55"/>
+    <mergeCell ref="G56:I56"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="L56:M56"/>
+    <mergeCell ref="G53:I53"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="L53:M53"/>
+    <mergeCell ref="G54:I54"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="L54:M54"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="L51:M51"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="L52:M52"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="L50:M50"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L9:M10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:I10"/>
+    <mergeCell ref="J9:K10"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
   </mergeCells>
   <conditionalFormatting sqref="B28:B71">
     <cfRule type="cellIs" dxfId="208" priority="213" stopIfTrue="1" operator="equal">
@@ -8737,452 +8737,452 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:99" ht="15" customHeight="1">
-      <c r="A2" s="135" t="s">
+      <c r="A2" s="167" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="135"/>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="135"/>
-      <c r="K2" s="135"/>
-      <c r="L2" s="135"/>
-      <c r="M2" s="135"/>
-      <c r="N2" s="135"/>
-      <c r="O2" s="135"/>
-      <c r="P2" s="135"/>
-      <c r="Q2" s="135"/>
-      <c r="R2" s="135"/>
-      <c r="S2" s="135"/>
-      <c r="T2" s="135"/>
-      <c r="U2" s="135"/>
-      <c r="V2" s="135"/>
-      <c r="W2" s="135"/>
-      <c r="X2" s="135"/>
-      <c r="Y2" s="135"/>
-      <c r="Z2" s="135"/>
-      <c r="AA2" s="135"/>
-      <c r="AB2" s="135"/>
-      <c r="AC2" s="135"/>
-      <c r="AD2" s="135"/>
-      <c r="AE2" s="135"/>
-      <c r="AF2" s="135"/>
-      <c r="AG2" s="135"/>
-      <c r="AH2" s="135"/>
-      <c r="AI2" s="135"/>
-      <c r="AJ2" s="135"/>
-      <c r="AK2" s="135"/>
-      <c r="AL2" s="135"/>
-      <c r="AM2" s="135"/>
-      <c r="AN2" s="135"/>
-      <c r="AO2" s="135"/>
-      <c r="AP2" s="135"/>
-      <c r="AQ2" s="135"/>
-      <c r="AR2" s="135"/>
-      <c r="AS2" s="135"/>
-      <c r="AT2" s="135"/>
-      <c r="AU2" s="135"/>
-      <c r="AV2" s="135"/>
-      <c r="AW2" s="135"/>
-      <c r="AX2" s="135"/>
-      <c r="AY2" s="135"/>
-      <c r="AZ2" s="135"/>
-      <c r="BA2" s="135"/>
-      <c r="BB2" s="135"/>
-      <c r="BC2" s="135"/>
-      <c r="BD2" s="135"/>
-      <c r="BE2" s="135"/>
-      <c r="BF2" s="135"/>
-      <c r="BG2" s="135"/>
-      <c r="BH2" s="135"/>
-      <c r="BI2" s="135"/>
-      <c r="BJ2" s="135"/>
-      <c r="BK2" s="135"/>
-      <c r="BL2" s="135"/>
-      <c r="BM2" s="135"/>
-      <c r="BN2" s="135"/>
-      <c r="BO2" s="135"/>
-      <c r="BP2" s="135"/>
-      <c r="BQ2" s="135"/>
-      <c r="BR2" s="135"/>
-      <c r="BS2" s="135"/>
-      <c r="BT2" s="135"/>
-      <c r="BU2" s="135"/>
-      <c r="BV2" s="135"/>
-      <c r="BW2" s="135"/>
-      <c r="BX2" s="135"/>
-      <c r="BY2" s="135"/>
-      <c r="BZ2" s="135"/>
-      <c r="CA2" s="135"/>
-      <c r="CB2" s="135"/>
-      <c r="CC2" s="135"/>
-      <c r="CD2" s="135"/>
-      <c r="CE2" s="135"/>
-      <c r="CF2" s="135"/>
-      <c r="CG2" s="135"/>
-      <c r="CH2" s="135"/>
-      <c r="CI2" s="135"/>
-      <c r="CJ2" s="135"/>
-      <c r="CK2" s="135"/>
-      <c r="CL2" s="135"/>
-      <c r="CM2" s="135"/>
-      <c r="CN2" s="135"/>
-      <c r="CO2" s="135"/>
-      <c r="CP2" s="135"/>
-      <c r="CQ2" s="135"/>
-      <c r="CR2" s="135"/>
-      <c r="CS2" s="135"/>
-      <c r="CT2" s="135"/>
-      <c r="CU2" s="135"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
+      <c r="P2" s="167"/>
+      <c r="Q2" s="167"/>
+      <c r="R2" s="167"/>
+      <c r="S2" s="167"/>
+      <c r="T2" s="167"/>
+      <c r="U2" s="167"/>
+      <c r="V2" s="167"/>
+      <c r="W2" s="167"/>
+      <c r="X2" s="167"/>
+      <c r="Y2" s="167"/>
+      <c r="Z2" s="167"/>
+      <c r="AA2" s="167"/>
+      <c r="AB2" s="167"/>
+      <c r="AC2" s="167"/>
+      <c r="AD2" s="167"/>
+      <c r="AE2" s="167"/>
+      <c r="AF2" s="167"/>
+      <c r="AG2" s="167"/>
+      <c r="AH2" s="167"/>
+      <c r="AI2" s="167"/>
+      <c r="AJ2" s="167"/>
+      <c r="AK2" s="167"/>
+      <c r="AL2" s="167"/>
+      <c r="AM2" s="167"/>
+      <c r="AN2" s="167"/>
+      <c r="AO2" s="167"/>
+      <c r="AP2" s="167"/>
+      <c r="AQ2" s="167"/>
+      <c r="AR2" s="167"/>
+      <c r="AS2" s="167"/>
+      <c r="AT2" s="167"/>
+      <c r="AU2" s="167"/>
+      <c r="AV2" s="167"/>
+      <c r="AW2" s="167"/>
+      <c r="AX2" s="167"/>
+      <c r="AY2" s="167"/>
+      <c r="AZ2" s="167"/>
+      <c r="BA2" s="167"/>
+      <c r="BB2" s="167"/>
+      <c r="BC2" s="167"/>
+      <c r="BD2" s="167"/>
+      <c r="BE2" s="167"/>
+      <c r="BF2" s="167"/>
+      <c r="BG2" s="167"/>
+      <c r="BH2" s="167"/>
+      <c r="BI2" s="167"/>
+      <c r="BJ2" s="167"/>
+      <c r="BK2" s="167"/>
+      <c r="BL2" s="167"/>
+      <c r="BM2" s="167"/>
+      <c r="BN2" s="167"/>
+      <c r="BO2" s="167"/>
+      <c r="BP2" s="167"/>
+      <c r="BQ2" s="167"/>
+      <c r="BR2" s="167"/>
+      <c r="BS2" s="167"/>
+      <c r="BT2" s="167"/>
+      <c r="BU2" s="167"/>
+      <c r="BV2" s="167"/>
+      <c r="BW2" s="167"/>
+      <c r="BX2" s="167"/>
+      <c r="BY2" s="167"/>
+      <c r="BZ2" s="167"/>
+      <c r="CA2" s="167"/>
+      <c r="CB2" s="167"/>
+      <c r="CC2" s="167"/>
+      <c r="CD2" s="167"/>
+      <c r="CE2" s="167"/>
+      <c r="CF2" s="167"/>
+      <c r="CG2" s="167"/>
+      <c r="CH2" s="167"/>
+      <c r="CI2" s="167"/>
+      <c r="CJ2" s="167"/>
+      <c r="CK2" s="167"/>
+      <c r="CL2" s="167"/>
+      <c r="CM2" s="167"/>
+      <c r="CN2" s="167"/>
+      <c r="CO2" s="167"/>
+      <c r="CP2" s="167"/>
+      <c r="CQ2" s="167"/>
+      <c r="CR2" s="167"/>
+      <c r="CS2" s="167"/>
+      <c r="CT2" s="167"/>
+      <c r="CU2" s="167"/>
     </row>
     <row r="3" spans="1:99" ht="15" customHeight="1">
-      <c r="A3" s="135"/>
-      <c r="B3" s="135"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135"/>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="135"/>
-      <c r="N3" s="135"/>
-      <c r="O3" s="135"/>
-      <c r="P3" s="135"/>
-      <c r="Q3" s="135"/>
-      <c r="R3" s="135"/>
-      <c r="S3" s="135"/>
-      <c r="T3" s="135"/>
-      <c r="U3" s="135"/>
-      <c r="V3" s="135"/>
-      <c r="W3" s="135"/>
-      <c r="X3" s="135"/>
-      <c r="Y3" s="135"/>
-      <c r="Z3" s="135"/>
-      <c r="AA3" s="135"/>
-      <c r="AB3" s="135"/>
-      <c r="AC3" s="135"/>
-      <c r="AD3" s="135"/>
-      <c r="AE3" s="135"/>
-      <c r="AF3" s="135"/>
-      <c r="AG3" s="135"/>
-      <c r="AH3" s="135"/>
-      <c r="AI3" s="135"/>
-      <c r="AJ3" s="135"/>
-      <c r="AK3" s="135"/>
-      <c r="AL3" s="135"/>
-      <c r="AM3" s="135"/>
-      <c r="AN3" s="135"/>
-      <c r="AO3" s="135"/>
-      <c r="AP3" s="135"/>
-      <c r="AQ3" s="135"/>
-      <c r="AR3" s="135"/>
-      <c r="AS3" s="135"/>
-      <c r="AT3" s="135"/>
-      <c r="AU3" s="135"/>
-      <c r="AV3" s="135"/>
-      <c r="AW3" s="135"/>
-      <c r="AX3" s="135"/>
-      <c r="AY3" s="135"/>
-      <c r="AZ3" s="135"/>
-      <c r="BA3" s="135"/>
-      <c r="BB3" s="135"/>
-      <c r="BC3" s="135"/>
-      <c r="BD3" s="135"/>
-      <c r="BE3" s="135"/>
-      <c r="BF3" s="135"/>
-      <c r="BG3" s="135"/>
-      <c r="BH3" s="135"/>
-      <c r="BI3" s="135"/>
-      <c r="BJ3" s="135"/>
-      <c r="BK3" s="135"/>
-      <c r="BL3" s="135"/>
-      <c r="BM3" s="135"/>
-      <c r="BN3" s="135"/>
-      <c r="BO3" s="135"/>
-      <c r="BP3" s="135"/>
-      <c r="BQ3" s="135"/>
-      <c r="BR3" s="135"/>
-      <c r="BS3" s="135"/>
-      <c r="BT3" s="135"/>
-      <c r="BU3" s="135"/>
-      <c r="BV3" s="135"/>
-      <c r="BW3" s="135"/>
-      <c r="BX3" s="135"/>
-      <c r="BY3" s="135"/>
-      <c r="BZ3" s="135"/>
-      <c r="CA3" s="135"/>
-      <c r="CB3" s="135"/>
-      <c r="CC3" s="135"/>
-      <c r="CD3" s="135"/>
-      <c r="CE3" s="135"/>
-      <c r="CF3" s="135"/>
-      <c r="CG3" s="135"/>
-      <c r="CH3" s="135"/>
-      <c r="CI3" s="135"/>
-      <c r="CJ3" s="135"/>
-      <c r="CK3" s="135"/>
-      <c r="CL3" s="135"/>
-      <c r="CM3" s="135"/>
-      <c r="CN3" s="135"/>
-      <c r="CO3" s="135"/>
-      <c r="CP3" s="135"/>
-      <c r="CQ3" s="135"/>
-      <c r="CR3" s="135"/>
-      <c r="CS3" s="135"/>
-      <c r="CT3" s="135"/>
-      <c r="CU3" s="135"/>
+      <c r="A3" s="167"/>
+      <c r="B3" s="167"/>
+      <c r="C3" s="167"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="167"/>
+      <c r="F3" s="167"/>
+      <c r="G3" s="167"/>
+      <c r="H3" s="167"/>
+      <c r="I3" s="167"/>
+      <c r="J3" s="167"/>
+      <c r="K3" s="167"/>
+      <c r="L3" s="167"/>
+      <c r="M3" s="167"/>
+      <c r="N3" s="167"/>
+      <c r="O3" s="167"/>
+      <c r="P3" s="167"/>
+      <c r="Q3" s="167"/>
+      <c r="R3" s="167"/>
+      <c r="S3" s="167"/>
+      <c r="T3" s="167"/>
+      <c r="U3" s="167"/>
+      <c r="V3" s="167"/>
+      <c r="W3" s="167"/>
+      <c r="X3" s="167"/>
+      <c r="Y3" s="167"/>
+      <c r="Z3" s="167"/>
+      <c r="AA3" s="167"/>
+      <c r="AB3" s="167"/>
+      <c r="AC3" s="167"/>
+      <c r="AD3" s="167"/>
+      <c r="AE3" s="167"/>
+      <c r="AF3" s="167"/>
+      <c r="AG3" s="167"/>
+      <c r="AH3" s="167"/>
+      <c r="AI3" s="167"/>
+      <c r="AJ3" s="167"/>
+      <c r="AK3" s="167"/>
+      <c r="AL3" s="167"/>
+      <c r="AM3" s="167"/>
+      <c r="AN3" s="167"/>
+      <c r="AO3" s="167"/>
+      <c r="AP3" s="167"/>
+      <c r="AQ3" s="167"/>
+      <c r="AR3" s="167"/>
+      <c r="AS3" s="167"/>
+      <c r="AT3" s="167"/>
+      <c r="AU3" s="167"/>
+      <c r="AV3" s="167"/>
+      <c r="AW3" s="167"/>
+      <c r="AX3" s="167"/>
+      <c r="AY3" s="167"/>
+      <c r="AZ3" s="167"/>
+      <c r="BA3" s="167"/>
+      <c r="BB3" s="167"/>
+      <c r="BC3" s="167"/>
+      <c r="BD3" s="167"/>
+      <c r="BE3" s="167"/>
+      <c r="BF3" s="167"/>
+      <c r="BG3" s="167"/>
+      <c r="BH3" s="167"/>
+      <c r="BI3" s="167"/>
+      <c r="BJ3" s="167"/>
+      <c r="BK3" s="167"/>
+      <c r="BL3" s="167"/>
+      <c r="BM3" s="167"/>
+      <c r="BN3" s="167"/>
+      <c r="BO3" s="167"/>
+      <c r="BP3" s="167"/>
+      <c r="BQ3" s="167"/>
+      <c r="BR3" s="167"/>
+      <c r="BS3" s="167"/>
+      <c r="BT3" s="167"/>
+      <c r="BU3" s="167"/>
+      <c r="BV3" s="167"/>
+      <c r="BW3" s="167"/>
+      <c r="BX3" s="167"/>
+      <c r="BY3" s="167"/>
+      <c r="BZ3" s="167"/>
+      <c r="CA3" s="167"/>
+      <c r="CB3" s="167"/>
+      <c r="CC3" s="167"/>
+      <c r="CD3" s="167"/>
+      <c r="CE3" s="167"/>
+      <c r="CF3" s="167"/>
+      <c r="CG3" s="167"/>
+      <c r="CH3" s="167"/>
+      <c r="CI3" s="167"/>
+      <c r="CJ3" s="167"/>
+      <c r="CK3" s="167"/>
+      <c r="CL3" s="167"/>
+      <c r="CM3" s="167"/>
+      <c r="CN3" s="167"/>
+      <c r="CO3" s="167"/>
+      <c r="CP3" s="167"/>
+      <c r="CQ3" s="167"/>
+      <c r="CR3" s="167"/>
+      <c r="CS3" s="167"/>
+      <c r="CT3" s="167"/>
+      <c r="CU3" s="167"/>
     </row>
     <row r="4" spans="1:99" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:99" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A5" s="200" t="s">
+      <c r="A5" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="203" t="s">
+      <c r="B5" s="178" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="203" t="s">
+      <c r="C5" s="178" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="204" t="s">
+      <c r="D5" s="179" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="205"/>
-      <c r="F5" s="205"/>
-      <c r="G5" s="205"/>
-      <c r="H5" s="205"/>
-      <c r="I5" s="205"/>
-      <c r="J5" s="205"/>
-      <c r="K5" s="205"/>
-      <c r="L5" s="205"/>
-      <c r="M5" s="205"/>
-      <c r="N5" s="205"/>
-      <c r="O5" s="205"/>
-      <c r="P5" s="205"/>
-      <c r="Q5" s="205"/>
-      <c r="R5" s="205"/>
-      <c r="S5" s="205"/>
-      <c r="T5" s="205"/>
-      <c r="U5" s="205"/>
-      <c r="V5" s="205"/>
-      <c r="W5" s="205"/>
-      <c r="X5" s="205"/>
-      <c r="Y5" s="205"/>
-      <c r="Z5" s="205"/>
-      <c r="AA5" s="205"/>
-      <c r="AB5" s="205"/>
-      <c r="AC5" s="205"/>
-      <c r="AD5" s="205"/>
-      <c r="AE5" s="205"/>
-      <c r="AF5" s="205"/>
-      <c r="AG5" s="205"/>
-      <c r="AH5" s="205"/>
-      <c r="AI5" s="205"/>
-      <c r="AJ5" s="205"/>
-      <c r="AK5" s="205"/>
-      <c r="AL5" s="205"/>
-      <c r="AM5" s="205"/>
-      <c r="AN5" s="205"/>
-      <c r="AO5" s="205"/>
-      <c r="AP5" s="205"/>
-      <c r="AQ5" s="205"/>
-      <c r="AR5" s="205"/>
-      <c r="AS5" s="205"/>
-      <c r="AT5" s="205"/>
-      <c r="AU5" s="205"/>
-      <c r="AV5" s="205"/>
-      <c r="AW5" s="205"/>
-      <c r="AX5" s="205"/>
-      <c r="AY5" s="205"/>
-      <c r="AZ5" s="205"/>
-      <c r="BA5" s="205"/>
-      <c r="BB5" s="205"/>
-      <c r="BC5" s="205"/>
-      <c r="BD5" s="206"/>
-      <c r="BE5" s="207" t="s">
+      <c r="E5" s="180"/>
+      <c r="F5" s="180"/>
+      <c r="G5" s="180"/>
+      <c r="H5" s="180"/>
+      <c r="I5" s="180"/>
+      <c r="J5" s="180"/>
+      <c r="K5" s="180"/>
+      <c r="L5" s="180"/>
+      <c r="M5" s="180"/>
+      <c r="N5" s="180"/>
+      <c r="O5" s="180"/>
+      <c r="P5" s="180"/>
+      <c r="Q5" s="180"/>
+      <c r="R5" s="180"/>
+      <c r="S5" s="180"/>
+      <c r="T5" s="180"/>
+      <c r="U5" s="180"/>
+      <c r="V5" s="180"/>
+      <c r="W5" s="180"/>
+      <c r="X5" s="180"/>
+      <c r="Y5" s="180"/>
+      <c r="Z5" s="180"/>
+      <c r="AA5" s="180"/>
+      <c r="AB5" s="180"/>
+      <c r="AC5" s="180"/>
+      <c r="AD5" s="180"/>
+      <c r="AE5" s="180"/>
+      <c r="AF5" s="180"/>
+      <c r="AG5" s="180"/>
+      <c r="AH5" s="180"/>
+      <c r="AI5" s="180"/>
+      <c r="AJ5" s="180"/>
+      <c r="AK5" s="180"/>
+      <c r="AL5" s="180"/>
+      <c r="AM5" s="180"/>
+      <c r="AN5" s="180"/>
+      <c r="AO5" s="180"/>
+      <c r="AP5" s="180"/>
+      <c r="AQ5" s="180"/>
+      <c r="AR5" s="180"/>
+      <c r="AS5" s="180"/>
+      <c r="AT5" s="180"/>
+      <c r="AU5" s="180"/>
+      <c r="AV5" s="180"/>
+      <c r="AW5" s="180"/>
+      <c r="AX5" s="180"/>
+      <c r="AY5" s="180"/>
+      <c r="AZ5" s="180"/>
+      <c r="BA5" s="180"/>
+      <c r="BB5" s="180"/>
+      <c r="BC5" s="180"/>
+      <c r="BD5" s="181"/>
+      <c r="BE5" s="182" t="s">
         <v>34</v>
       </c>
-      <c r="BF5" s="208"/>
-      <c r="BG5" s="208"/>
-      <c r="BH5" s="208"/>
-      <c r="BI5" s="208"/>
-      <c r="BJ5" s="208"/>
-      <c r="BK5" s="208"/>
-      <c r="BL5" s="208"/>
-      <c r="BM5" s="208"/>
-      <c r="BN5" s="208"/>
-      <c r="BO5" s="208"/>
-      <c r="BP5" s="208"/>
-      <c r="BQ5" s="208"/>
-      <c r="BR5" s="208"/>
-      <c r="BS5" s="208"/>
-      <c r="BT5" s="208"/>
-      <c r="BU5" s="208"/>
-      <c r="BV5" s="208"/>
-      <c r="BW5" s="208"/>
-      <c r="BX5" s="208"/>
-      <c r="BY5" s="208"/>
-      <c r="BZ5" s="208"/>
-      <c r="CA5" s="208"/>
-      <c r="CB5" s="208"/>
-      <c r="CC5" s="208"/>
-      <c r="CD5" s="208"/>
-      <c r="CE5" s="208"/>
-      <c r="CF5" s="208"/>
-      <c r="CG5" s="208"/>
-      <c r="CH5" s="208"/>
-      <c r="CI5" s="208"/>
-      <c r="CJ5" s="208"/>
-      <c r="CK5" s="208"/>
-      <c r="CL5" s="208"/>
-      <c r="CM5" s="208"/>
-      <c r="CN5" s="208"/>
-      <c r="CO5" s="208"/>
-      <c r="CP5" s="208"/>
-      <c r="CQ5" s="208"/>
-      <c r="CR5" s="209"/>
-      <c r="CS5" s="196" t="s">
+      <c r="BF5" s="183"/>
+      <c r="BG5" s="183"/>
+      <c r="BH5" s="183"/>
+      <c r="BI5" s="183"/>
+      <c r="BJ5" s="183"/>
+      <c r="BK5" s="183"/>
+      <c r="BL5" s="183"/>
+      <c r="BM5" s="183"/>
+      <c r="BN5" s="183"/>
+      <c r="BO5" s="183"/>
+      <c r="BP5" s="183"/>
+      <c r="BQ5" s="183"/>
+      <c r="BR5" s="183"/>
+      <c r="BS5" s="183"/>
+      <c r="BT5" s="183"/>
+      <c r="BU5" s="183"/>
+      <c r="BV5" s="183"/>
+      <c r="BW5" s="183"/>
+      <c r="BX5" s="183"/>
+      <c r="BY5" s="183"/>
+      <c r="BZ5" s="183"/>
+      <c r="CA5" s="183"/>
+      <c r="CB5" s="183"/>
+      <c r="CC5" s="183"/>
+      <c r="CD5" s="183"/>
+      <c r="CE5" s="183"/>
+      <c r="CF5" s="183"/>
+      <c r="CG5" s="183"/>
+      <c r="CH5" s="183"/>
+      <c r="CI5" s="183"/>
+      <c r="CJ5" s="183"/>
+      <c r="CK5" s="183"/>
+      <c r="CL5" s="183"/>
+      <c r="CM5" s="183"/>
+      <c r="CN5" s="183"/>
+      <c r="CO5" s="183"/>
+      <c r="CP5" s="183"/>
+      <c r="CQ5" s="183"/>
+      <c r="CR5" s="184"/>
+      <c r="CS5" s="189" t="s">
         <v>35</v>
       </c>
-      <c r="CT5" s="197"/>
-      <c r="CU5" s="198"/>
+      <c r="CT5" s="190"/>
+      <c r="CU5" s="191"/>
     </row>
     <row r="6" spans="1:99" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A6" s="201"/>
-      <c r="B6" s="203"/>
-      <c r="C6" s="203"/>
-      <c r="D6" s="179" t="s">
+      <c r="A6" s="176"/>
+      <c r="B6" s="178"/>
+      <c r="C6" s="178"/>
+      <c r="D6" s="209" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="180"/>
-      <c r="F6" s="180"/>
-      <c r="G6" s="180"/>
-      <c r="H6" s="180"/>
-      <c r="I6" s="180"/>
-      <c r="J6" s="182" t="s">
+      <c r="E6" s="210"/>
+      <c r="F6" s="210"/>
+      <c r="G6" s="210"/>
+      <c r="H6" s="210"/>
+      <c r="I6" s="210"/>
+      <c r="J6" s="195" t="s">
         <v>140</v>
       </c>
-      <c r="K6" s="182"/>
-      <c r="L6" s="182"/>
-      <c r="M6" s="182"/>
-      <c r="N6" s="182"/>
-      <c r="O6" s="182"/>
-      <c r="P6" s="182"/>
-      <c r="Q6" s="182"/>
-      <c r="R6" s="182"/>
-      <c r="S6" s="182"/>
-      <c r="T6" s="182"/>
-      <c r="U6" s="182"/>
-      <c r="V6" s="182"/>
-      <c r="W6" s="182"/>
-      <c r="X6" s="182"/>
-      <c r="Y6" s="182"/>
-      <c r="Z6" s="182"/>
-      <c r="AA6" s="182"/>
-      <c r="AB6" s="182"/>
-      <c r="AC6" s="182"/>
-      <c r="AD6" s="182"/>
-      <c r="AE6" s="182"/>
-      <c r="AF6" s="182"/>
-      <c r="AG6" s="182"/>
-      <c r="AH6" s="182"/>
-      <c r="AI6" s="182"/>
-      <c r="AJ6" s="182"/>
-      <c r="AK6" s="182"/>
-      <c r="AL6" s="182"/>
-      <c r="AM6" s="182"/>
-      <c r="AN6" s="182"/>
-      <c r="AO6" s="182" t="s">
+      <c r="K6" s="195"/>
+      <c r="L6" s="195"/>
+      <c r="M6" s="195"/>
+      <c r="N6" s="195"/>
+      <c r="O6" s="195"/>
+      <c r="P6" s="195"/>
+      <c r="Q6" s="195"/>
+      <c r="R6" s="195"/>
+      <c r="S6" s="195"/>
+      <c r="T6" s="195"/>
+      <c r="U6" s="195"/>
+      <c r="V6" s="195"/>
+      <c r="W6" s="195"/>
+      <c r="X6" s="195"/>
+      <c r="Y6" s="195"/>
+      <c r="Z6" s="195"/>
+      <c r="AA6" s="195"/>
+      <c r="AB6" s="195"/>
+      <c r="AC6" s="195"/>
+      <c r="AD6" s="195"/>
+      <c r="AE6" s="195"/>
+      <c r="AF6" s="195"/>
+      <c r="AG6" s="195"/>
+      <c r="AH6" s="195"/>
+      <c r="AI6" s="195"/>
+      <c r="AJ6" s="195"/>
+      <c r="AK6" s="195"/>
+      <c r="AL6" s="195"/>
+      <c r="AM6" s="195"/>
+      <c r="AN6" s="195"/>
+      <c r="AO6" s="195" t="s">
         <v>141</v>
       </c>
-      <c r="AP6" s="182"/>
-      <c r="AQ6" s="182"/>
-      <c r="AR6" s="182"/>
-      <c r="AS6" s="182" t="s">
+      <c r="AP6" s="195"/>
+      <c r="AQ6" s="195"/>
+      <c r="AR6" s="195"/>
+      <c r="AS6" s="195" t="s">
         <v>37</v>
       </c>
-      <c r="AT6" s="182"/>
-      <c r="AU6" s="182"/>
-      <c r="AV6" s="182" t="s">
+      <c r="AT6" s="195"/>
+      <c r="AU6" s="195"/>
+      <c r="AV6" s="195" t="s">
         <v>38</v>
       </c>
-      <c r="AW6" s="182"/>
-      <c r="AX6" s="182"/>
-      <c r="AY6" s="182"/>
-      <c r="AZ6" s="182"/>
-      <c r="BA6" s="182"/>
-      <c r="BB6" s="182"/>
-      <c r="BC6" s="189" t="s">
+      <c r="AW6" s="195"/>
+      <c r="AX6" s="195"/>
+      <c r="AY6" s="195"/>
+      <c r="AZ6" s="195"/>
+      <c r="BA6" s="195"/>
+      <c r="BB6" s="195"/>
+      <c r="BC6" s="199" t="s">
         <v>39</v>
       </c>
-      <c r="BD6" s="190"/>
-      <c r="BE6" s="191" t="s">
+      <c r="BD6" s="200"/>
+      <c r="BE6" s="201" t="s">
         <v>102</v>
       </c>
-      <c r="BF6" s="192"/>
-      <c r="BG6" s="192"/>
-      <c r="BH6" s="192"/>
-      <c r="BI6" s="192"/>
-      <c r="BJ6" s="192"/>
-      <c r="BK6" s="193"/>
-      <c r="BL6" s="194" t="s">
+      <c r="BF6" s="202"/>
+      <c r="BG6" s="202"/>
+      <c r="BH6" s="202"/>
+      <c r="BI6" s="202"/>
+      <c r="BJ6" s="202"/>
+      <c r="BK6" s="203"/>
+      <c r="BL6" s="204" t="s">
         <v>103</v>
       </c>
-      <c r="BM6" s="192"/>
-      <c r="BN6" s="192"/>
-      <c r="BO6" s="192"/>
-      <c r="BP6" s="192"/>
-      <c r="BQ6" s="192"/>
-      <c r="BR6" s="192"/>
-      <c r="BS6" s="192"/>
-      <c r="BT6" s="192"/>
-      <c r="BU6" s="192"/>
-      <c r="BV6" s="192"/>
-      <c r="BW6" s="192"/>
-      <c r="BX6" s="192"/>
-      <c r="BY6" s="192"/>
-      <c r="BZ6" s="192"/>
-      <c r="CA6" s="192"/>
-      <c r="CB6" s="192"/>
-      <c r="CC6" s="192"/>
-      <c r="CD6" s="192"/>
-      <c r="CE6" s="192"/>
-      <c r="CF6" s="192"/>
-      <c r="CG6" s="192"/>
-      <c r="CH6" s="192"/>
-      <c r="CI6" s="192"/>
-      <c r="CJ6" s="192"/>
-      <c r="CK6" s="192"/>
-      <c r="CL6" s="192"/>
-      <c r="CM6" s="192"/>
-      <c r="CN6" s="192"/>
-      <c r="CO6" s="192"/>
-      <c r="CP6" s="192"/>
-      <c r="CQ6" s="199" t="s">
+      <c r="BM6" s="202"/>
+      <c r="BN6" s="202"/>
+      <c r="BO6" s="202"/>
+      <c r="BP6" s="202"/>
+      <c r="BQ6" s="202"/>
+      <c r="BR6" s="202"/>
+      <c r="BS6" s="202"/>
+      <c r="BT6" s="202"/>
+      <c r="BU6" s="202"/>
+      <c r="BV6" s="202"/>
+      <c r="BW6" s="202"/>
+      <c r="BX6" s="202"/>
+      <c r="BY6" s="202"/>
+      <c r="BZ6" s="202"/>
+      <c r="CA6" s="202"/>
+      <c r="CB6" s="202"/>
+      <c r="CC6" s="202"/>
+      <c r="CD6" s="202"/>
+      <c r="CE6" s="202"/>
+      <c r="CF6" s="202"/>
+      <c r="CG6" s="202"/>
+      <c r="CH6" s="202"/>
+      <c r="CI6" s="202"/>
+      <c r="CJ6" s="202"/>
+      <c r="CK6" s="202"/>
+      <c r="CL6" s="202"/>
+      <c r="CM6" s="202"/>
+      <c r="CN6" s="202"/>
+      <c r="CO6" s="202"/>
+      <c r="CP6" s="202"/>
+      <c r="CQ6" s="192" t="s">
         <v>40</v>
       </c>
-      <c r="CR6" s="199"/>
-      <c r="CS6" s="195" t="s">
+      <c r="CR6" s="192"/>
+      <c r="CS6" s="174" t="s">
         <v>41</v>
       </c>
-      <c r="CT6" s="195" t="s">
+      <c r="CT6" s="174" t="s">
         <v>42</v>
       </c>
-      <c r="CU6" s="186" t="s">
+      <c r="CU6" s="196" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:99" ht="15.75" thickBot="1">
-      <c r="A7" s="201"/>
-      <c r="B7" s="203"/>
-      <c r="C7" s="203"/>
+      <c r="A7" s="176"/>
+      <c r="B7" s="178"/>
+      <c r="C7" s="178"/>
       <c r="E7" s="123"/>
       <c r="F7" s="122">
         <v>0.3</v>
@@ -9191,339 +9191,339 @@
       <c r="I7" s="123">
         <v>0.3</v>
       </c>
-      <c r="J7" s="181">
+      <c r="J7" s="187">
         <v>42983</v>
       </c>
-      <c r="K7" s="181"/>
-      <c r="L7" s="181">
+      <c r="K7" s="187"/>
+      <c r="L7" s="187">
         <v>43004</v>
       </c>
-      <c r="M7" s="181"/>
-      <c r="N7" s="181"/>
-      <c r="O7" s="181"/>
-      <c r="P7" s="181"/>
-      <c r="Q7" s="181"/>
-      <c r="R7" s="181"/>
-      <c r="S7" s="181"/>
-      <c r="T7" s="185">
+      <c r="M7" s="187"/>
+      <c r="N7" s="187"/>
+      <c r="O7" s="187"/>
+      <c r="P7" s="187"/>
+      <c r="Q7" s="187"/>
+      <c r="R7" s="187"/>
+      <c r="S7" s="187"/>
+      <c r="T7" s="188">
         <f>COUNT(J9,L9,N9,P9,R9,T9)</f>
         <v>2</v>
       </c>
-      <c r="U7" s="185"/>
-      <c r="V7" s="181"/>
-      <c r="W7" s="181"/>
-      <c r="X7" s="181"/>
-      <c r="Y7" s="181"/>
-      <c r="Z7" s="181"/>
-      <c r="AA7" s="181"/>
-      <c r="AB7" s="181"/>
-      <c r="AC7" s="181"/>
-      <c r="AD7" s="181"/>
-      <c r="AE7" s="181"/>
-      <c r="AF7" s="181"/>
-      <c r="AG7" s="181"/>
-      <c r="AH7" s="181"/>
-      <c r="AI7" s="181"/>
-      <c r="AJ7" s="181"/>
-      <c r="AK7" s="181"/>
-      <c r="AL7" s="181"/>
-      <c r="AM7" s="181"/>
+      <c r="U7" s="188"/>
+      <c r="V7" s="187"/>
+      <c r="W7" s="187"/>
+      <c r="X7" s="187"/>
+      <c r="Y7" s="187"/>
+      <c r="Z7" s="187"/>
+      <c r="AA7" s="187"/>
+      <c r="AB7" s="187"/>
+      <c r="AC7" s="187"/>
+      <c r="AD7" s="187"/>
+      <c r="AE7" s="187"/>
+      <c r="AF7" s="187"/>
+      <c r="AG7" s="187"/>
+      <c r="AH7" s="187"/>
+      <c r="AI7" s="187"/>
+      <c r="AJ7" s="187"/>
+      <c r="AK7" s="187"/>
+      <c r="AL7" s="187"/>
+      <c r="AM7" s="187"/>
       <c r="AN7" s="96">
         <v>0.2</v>
       </c>
-      <c r="AO7" s="181" t="s">
+      <c r="AO7" s="187" t="s">
         <v>166</v>
       </c>
-      <c r="AP7" s="181"/>
-      <c r="AQ7" s="181"/>
-      <c r="AR7" s="181"/>
-      <c r="AS7" s="185">
+      <c r="AP7" s="187"/>
+      <c r="AQ7" s="187"/>
+      <c r="AR7" s="187"/>
+      <c r="AS7" s="188">
         <f>COUNT(AO9,AQ9,AS9)</f>
         <v>1</v>
       </c>
-      <c r="AT7" s="185"/>
+      <c r="AT7" s="188"/>
       <c r="AU7" s="20">
         <v>0.1</v>
       </c>
-      <c r="AV7" s="181" t="s">
+      <c r="AV7" s="187" t="s">
         <v>167</v>
       </c>
-      <c r="AW7" s="181"/>
-      <c r="AX7" s="181"/>
-      <c r="AY7" s="181"/>
-      <c r="AZ7" s="185">
+      <c r="AW7" s="187"/>
+      <c r="AX7" s="187"/>
+      <c r="AY7" s="187"/>
+      <c r="AZ7" s="188">
         <f>COUNT(AV9,AX9,AZ9)</f>
         <v>1</v>
       </c>
-      <c r="BA7" s="185"/>
+      <c r="BA7" s="188"/>
       <c r="BB7" s="21">
         <v>0.1</v>
       </c>
-      <c r="BC7" s="189"/>
-      <c r="BD7" s="190"/>
-      <c r="BE7" s="181" t="s">
+      <c r="BC7" s="199"/>
+      <c r="BD7" s="200"/>
+      <c r="BE7" s="187" t="s">
         <v>339</v>
       </c>
-      <c r="BF7" s="181"/>
-      <c r="BG7" s="181" t="s">
+      <c r="BF7" s="187"/>
+      <c r="BG7" s="187" t="s">
         <v>338</v>
       </c>
-      <c r="BH7" s="181"/>
-      <c r="BI7" s="185">
+      <c r="BH7" s="187"/>
+      <c r="BI7" s="188">
         <f>COUNT(BE9,BG9,BI9)</f>
         <v>2</v>
       </c>
-      <c r="BJ7" s="185"/>
+      <c r="BJ7" s="188"/>
       <c r="BK7" s="104">
         <v>0.5</v>
       </c>
-      <c r="BL7" s="181">
+      <c r="BL7" s="187">
         <v>42982</v>
       </c>
-      <c r="BM7" s="181"/>
-      <c r="BN7" s="181">
+      <c r="BM7" s="187"/>
+      <c r="BN7" s="187">
         <v>42982</v>
       </c>
-      <c r="BO7" s="181"/>
-      <c r="BP7" s="181">
+      <c r="BO7" s="187"/>
+      <c r="BP7" s="187">
         <v>42989</v>
       </c>
-      <c r="BQ7" s="181"/>
-      <c r="BR7" s="181">
+      <c r="BQ7" s="187"/>
+      <c r="BR7" s="187">
         <v>42987</v>
       </c>
-      <c r="BS7" s="181"/>
-      <c r="BT7" s="181"/>
-      <c r="BU7" s="181"/>
-      <c r="BV7" s="181"/>
-      <c r="BW7" s="181"/>
-      <c r="BX7" s="181"/>
-      <c r="BY7" s="181"/>
-      <c r="BZ7" s="181"/>
-      <c r="CA7" s="181"/>
-      <c r="CB7" s="181"/>
-      <c r="CC7" s="181"/>
-      <c r="CD7" s="181"/>
-      <c r="CE7" s="181"/>
-      <c r="CF7" s="181"/>
-      <c r="CG7" s="181"/>
-      <c r="CH7" s="181"/>
-      <c r="CI7" s="181"/>
-      <c r="CJ7" s="181"/>
-      <c r="CK7" s="181"/>
-      <c r="CL7" s="181"/>
-      <c r="CM7" s="181"/>
-      <c r="CN7" s="185">
+      <c r="BS7" s="187"/>
+      <c r="BT7" s="187"/>
+      <c r="BU7" s="187"/>
+      <c r="BV7" s="187"/>
+      <c r="BW7" s="187"/>
+      <c r="BX7" s="187"/>
+      <c r="BY7" s="187"/>
+      <c r="BZ7" s="187"/>
+      <c r="CA7" s="187"/>
+      <c r="CB7" s="187"/>
+      <c r="CC7" s="187"/>
+      <c r="CD7" s="187"/>
+      <c r="CE7" s="187"/>
+      <c r="CF7" s="187"/>
+      <c r="CG7" s="187"/>
+      <c r="CH7" s="187"/>
+      <c r="CI7" s="187"/>
+      <c r="CJ7" s="187"/>
+      <c r="CK7" s="187"/>
+      <c r="CL7" s="187"/>
+      <c r="CM7" s="187"/>
+      <c r="CN7" s="188">
         <f>COUNT(CN9,CL9,CJ9,CH9,CF9,CD9,CB9,BZ9,BX9,BV9,BT9,BR9,BP9,BN9,BL9)</f>
         <v>3</v>
       </c>
-      <c r="CO7" s="185"/>
+      <c r="CO7" s="188"/>
       <c r="CP7" s="105">
         <v>0.5</v>
       </c>
-      <c r="CQ7" s="199"/>
-      <c r="CR7" s="199"/>
-      <c r="CS7" s="195"/>
-      <c r="CT7" s="195"/>
-      <c r="CU7" s="187"/>
+      <c r="CQ7" s="192"/>
+      <c r="CR7" s="192"/>
+      <c r="CS7" s="174"/>
+      <c r="CT7" s="174"/>
+      <c r="CU7" s="197"/>
     </row>
     <row r="8" spans="1:99" ht="15.75" thickBot="1">
-      <c r="A8" s="201"/>
-      <c r="B8" s="203"/>
-      <c r="C8" s="203"/>
-      <c r="D8" s="210" t="s">
+      <c r="A8" s="176"/>
+      <c r="B8" s="178"/>
+      <c r="C8" s="178"/>
+      <c r="D8" s="185" t="s">
         <v>157</v>
       </c>
-      <c r="E8" s="210"/>
-      <c r="F8" s="210"/>
-      <c r="G8" s="210" t="s">
+      <c r="E8" s="185"/>
+      <c r="F8" s="185"/>
+      <c r="G8" s="185" t="s">
         <v>158</v>
       </c>
-      <c r="H8" s="210"/>
-      <c r="I8" s="210"/>
-      <c r="J8" s="174" t="s">
+      <c r="H8" s="185"/>
+      <c r="I8" s="185"/>
+      <c r="J8" s="186" t="s">
         <v>48</v>
       </c>
-      <c r="K8" s="174"/>
-      <c r="L8" s="174" t="s">
+      <c r="K8" s="186"/>
+      <c r="L8" s="186" t="s">
         <v>49</v>
       </c>
-      <c r="M8" s="174"/>
-      <c r="N8" s="174" t="s">
+      <c r="M8" s="186"/>
+      <c r="N8" s="186" t="s">
         <v>50</v>
       </c>
-      <c r="O8" s="174"/>
-      <c r="P8" s="174" t="s">
+      <c r="O8" s="186"/>
+      <c r="P8" s="186" t="s">
         <v>51</v>
       </c>
-      <c r="Q8" s="174"/>
-      <c r="R8" s="174" t="s">
+      <c r="Q8" s="186"/>
+      <c r="R8" s="186" t="s">
         <v>52</v>
       </c>
-      <c r="S8" s="174"/>
-      <c r="T8" s="174" t="s">
+      <c r="S8" s="186"/>
+      <c r="T8" s="186" t="s">
         <v>53</v>
       </c>
-      <c r="U8" s="174"/>
-      <c r="V8" s="174" t="s">
+      <c r="U8" s="186"/>
+      <c r="V8" s="186" t="s">
         <v>54</v>
       </c>
-      <c r="W8" s="174"/>
-      <c r="X8" s="174" t="s">
+      <c r="W8" s="186"/>
+      <c r="X8" s="186" t="s">
         <v>55</v>
       </c>
-      <c r="Y8" s="174"/>
-      <c r="Z8" s="174" t="s">
+      <c r="Y8" s="186"/>
+      <c r="Z8" s="186" t="s">
         <v>56</v>
       </c>
-      <c r="AA8" s="174"/>
-      <c r="AB8" s="174" t="s">
+      <c r="AA8" s="186"/>
+      <c r="AB8" s="186" t="s">
         <v>57</v>
       </c>
-      <c r="AC8" s="174"/>
-      <c r="AD8" s="174" t="s">
+      <c r="AC8" s="186"/>
+      <c r="AD8" s="186" t="s">
         <v>58</v>
       </c>
-      <c r="AE8" s="174"/>
-      <c r="AF8" s="174" t="s">
+      <c r="AE8" s="186"/>
+      <c r="AF8" s="186" t="s">
         <v>59</v>
       </c>
-      <c r="AG8" s="174"/>
-      <c r="AH8" s="174" t="s">
+      <c r="AG8" s="186"/>
+      <c r="AH8" s="186" t="s">
         <v>60</v>
       </c>
-      <c r="AI8" s="174"/>
-      <c r="AJ8" s="174" t="s">
+      <c r="AI8" s="186"/>
+      <c r="AJ8" s="186" t="s">
         <v>61</v>
       </c>
-      <c r="AK8" s="174"/>
-      <c r="AL8" s="174" t="s">
+      <c r="AK8" s="186"/>
+      <c r="AL8" s="186" t="s">
         <v>62</v>
       </c>
-      <c r="AM8" s="174"/>
+      <c r="AM8" s="186"/>
       <c r="AN8" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="AO8" s="174" t="s">
+      <c r="AO8" s="186" t="s">
         <v>64</v>
       </c>
-      <c r="AP8" s="174"/>
-      <c r="AQ8" s="174" t="s">
+      <c r="AP8" s="186"/>
+      <c r="AQ8" s="186" t="s">
         <v>65</v>
       </c>
-      <c r="AR8" s="174"/>
-      <c r="AS8" s="174" t="s">
+      <c r="AR8" s="186"/>
+      <c r="AS8" s="186" t="s">
         <v>66</v>
       </c>
-      <c r="AT8" s="174"/>
+      <c r="AT8" s="186"/>
       <c r="AU8" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="AV8" s="174" t="s">
+      <c r="AV8" s="186" t="s">
         <v>68</v>
       </c>
-      <c r="AW8" s="174"/>
-      <c r="AX8" s="174" t="s">
+      <c r="AW8" s="186"/>
+      <c r="AX8" s="186" t="s">
         <v>69</v>
       </c>
-      <c r="AY8" s="174"/>
-      <c r="AZ8" s="174" t="s">
+      <c r="AY8" s="186"/>
+      <c r="AZ8" s="186" t="s">
         <v>70</v>
       </c>
-      <c r="BA8" s="174"/>
+      <c r="BA8" s="186"/>
       <c r="BB8" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="BC8" s="189"/>
-      <c r="BD8" s="190"/>
-      <c r="BE8" s="184" t="s">
+      <c r="BC8" s="199"/>
+      <c r="BD8" s="200"/>
+      <c r="BE8" s="208" t="s">
         <v>44</v>
       </c>
-      <c r="BF8" s="183"/>
-      <c r="BG8" s="183" t="s">
+      <c r="BF8" s="205"/>
+      <c r="BG8" s="205" t="s">
         <v>45</v>
       </c>
-      <c r="BH8" s="183"/>
-      <c r="BI8" s="183" t="s">
+      <c r="BH8" s="205"/>
+      <c r="BI8" s="205" t="s">
         <v>46</v>
       </c>
-      <c r="BJ8" s="183"/>
+      <c r="BJ8" s="205"/>
       <c r="BK8" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="BL8" s="177" t="s">
+      <c r="BL8" s="206" t="s">
         <v>72</v>
       </c>
-      <c r="BM8" s="178"/>
-      <c r="BN8" s="177" t="s">
+      <c r="BM8" s="207"/>
+      <c r="BN8" s="206" t="s">
         <v>73</v>
       </c>
-      <c r="BO8" s="178"/>
-      <c r="BP8" s="177" t="s">
+      <c r="BO8" s="207"/>
+      <c r="BP8" s="206" t="s">
         <v>74</v>
       </c>
-      <c r="BQ8" s="178"/>
-      <c r="BR8" s="177" t="s">
+      <c r="BQ8" s="207"/>
+      <c r="BR8" s="206" t="s">
         <v>75</v>
       </c>
-      <c r="BS8" s="178"/>
-      <c r="BT8" s="177" t="s">
+      <c r="BS8" s="207"/>
+      <c r="BT8" s="206" t="s">
         <v>76</v>
       </c>
-      <c r="BU8" s="178"/>
-      <c r="BV8" s="175" t="s">
+      <c r="BU8" s="207"/>
+      <c r="BV8" s="193" t="s">
         <v>77</v>
       </c>
-      <c r="BW8" s="176"/>
-      <c r="BX8" s="175" t="s">
+      <c r="BW8" s="194"/>
+      <c r="BX8" s="193" t="s">
         <v>78</v>
       </c>
-      <c r="BY8" s="176"/>
-      <c r="BZ8" s="175" t="s">
+      <c r="BY8" s="194"/>
+      <c r="BZ8" s="193" t="s">
         <v>79</v>
       </c>
-      <c r="CA8" s="176"/>
-      <c r="CB8" s="175" t="s">
+      <c r="CA8" s="194"/>
+      <c r="CB8" s="193" t="s">
         <v>80</v>
       </c>
-      <c r="CC8" s="176"/>
-      <c r="CD8" s="175" t="s">
+      <c r="CC8" s="194"/>
+      <c r="CD8" s="193" t="s">
         <v>81</v>
       </c>
-      <c r="CE8" s="176"/>
-      <c r="CF8" s="175" t="s">
+      <c r="CE8" s="194"/>
+      <c r="CF8" s="193" t="s">
         <v>82</v>
       </c>
-      <c r="CG8" s="176"/>
-      <c r="CH8" s="175" t="s">
+      <c r="CG8" s="194"/>
+      <c r="CH8" s="193" t="s">
         <v>83</v>
       </c>
-      <c r="CI8" s="176"/>
-      <c r="CJ8" s="175" t="s">
+      <c r="CI8" s="194"/>
+      <c r="CJ8" s="193" t="s">
         <v>84</v>
       </c>
-      <c r="CK8" s="176"/>
-      <c r="CL8" s="175" t="s">
+      <c r="CK8" s="194"/>
+      <c r="CL8" s="193" t="s">
         <v>85</v>
       </c>
-      <c r="CM8" s="176"/>
-      <c r="CN8" s="175" t="s">
+      <c r="CM8" s="194"/>
+      <c r="CN8" s="193" t="s">
         <v>86</v>
       </c>
-      <c r="CO8" s="176"/>
+      <c r="CO8" s="194"/>
       <c r="CP8" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="CQ8" s="199"/>
-      <c r="CR8" s="199"/>
-      <c r="CS8" s="195"/>
-      <c r="CT8" s="195"/>
-      <c r="CU8" s="187"/>
+      <c r="CQ8" s="192"/>
+      <c r="CR8" s="192"/>
+      <c r="CS8" s="174"/>
+      <c r="CT8" s="174"/>
+      <c r="CU8" s="197"/>
     </row>
     <row r="9" spans="1:99" ht="15.75" thickBot="1">
-      <c r="A9" s="202"/>
-      <c r="B9" s="203"/>
-      <c r="C9" s="203"/>
+      <c r="A9" s="177"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="178"/>
       <c r="D9" s="26">
         <v>70</v>
       </c>
@@ -9697,9 +9697,9 @@
       <c r="CR9" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="CS9" s="195"/>
-      <c r="CT9" s="195"/>
-      <c r="CU9" s="188"/>
+      <c r="CS9" s="174"/>
+      <c r="CT9" s="174"/>
+      <c r="CU9" s="198"/>
     </row>
     <row r="10" spans="1:99">
       <c r="A10" s="41">
@@ -25394,6 +25394,88 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="98">
+    <mergeCell ref="AD8:AE8"/>
+    <mergeCell ref="AJ8:AK8"/>
+    <mergeCell ref="AV8:AW8"/>
+    <mergeCell ref="AX8:AY8"/>
+    <mergeCell ref="A2:CU3"/>
+    <mergeCell ref="CB8:CC8"/>
+    <mergeCell ref="CD8:CE8"/>
+    <mergeCell ref="CF8:CG8"/>
+    <mergeCell ref="CH8:CI8"/>
+    <mergeCell ref="CJ8:CK8"/>
+    <mergeCell ref="CL8:CM8"/>
+    <mergeCell ref="BP8:BQ8"/>
+    <mergeCell ref="BR8:BS8"/>
+    <mergeCell ref="BT8:BU8"/>
+    <mergeCell ref="BV8:BW8"/>
+    <mergeCell ref="BX8:BY8"/>
+    <mergeCell ref="BZ8:CA8"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="X8:Y8"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="AB8:AC8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="J6:AN6"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="AF8:AG8"/>
+    <mergeCell ref="AH8:AI8"/>
+    <mergeCell ref="BI8:BJ8"/>
+    <mergeCell ref="BL8:BM8"/>
+    <mergeCell ref="BN8:BO8"/>
+    <mergeCell ref="AL8:AM8"/>
+    <mergeCell ref="AO8:AP8"/>
+    <mergeCell ref="AQ8:AR8"/>
+    <mergeCell ref="AS8:AT8"/>
+    <mergeCell ref="BE8:BF8"/>
+    <mergeCell ref="AZ8:BA8"/>
+    <mergeCell ref="BG8:BH8"/>
+    <mergeCell ref="BI7:BJ7"/>
+    <mergeCell ref="AH7:AI7"/>
+    <mergeCell ref="AJ7:AK7"/>
+    <mergeCell ref="AL7:AM7"/>
+    <mergeCell ref="AO7:AP7"/>
+    <mergeCell ref="AQ7:AR7"/>
+    <mergeCell ref="AS7:AT7"/>
+    <mergeCell ref="AO6:AU6"/>
+    <mergeCell ref="AV6:BB6"/>
+    <mergeCell ref="CU6:CU9"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="BC6:BD8"/>
+    <mergeCell ref="BE6:BK6"/>
+    <mergeCell ref="BL6:CP6"/>
+    <mergeCell ref="AD7:AE7"/>
+    <mergeCell ref="AF7:AG7"/>
+    <mergeCell ref="CT6:CT9"/>
+    <mergeCell ref="BE7:BF7"/>
+    <mergeCell ref="CS5:CU5"/>
+    <mergeCell ref="BL7:BM7"/>
+    <mergeCell ref="BN7:BO7"/>
+    <mergeCell ref="BP7:BQ7"/>
+    <mergeCell ref="BR7:BS7"/>
+    <mergeCell ref="CL7:CM7"/>
+    <mergeCell ref="CN7:CO7"/>
+    <mergeCell ref="BT7:BU7"/>
+    <mergeCell ref="BV7:BW7"/>
+    <mergeCell ref="BX7:BY7"/>
+    <mergeCell ref="BZ7:CA7"/>
+    <mergeCell ref="CB7:CC7"/>
+    <mergeCell ref="CJ7:CK7"/>
+    <mergeCell ref="CD7:CE7"/>
+    <mergeCell ref="CQ6:CR8"/>
+    <mergeCell ref="CN8:CO8"/>
     <mergeCell ref="CS6:CS9"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="B5:B9"/>
@@ -25410,88 +25492,6 @@
     <mergeCell ref="BG7:BH7"/>
     <mergeCell ref="CF7:CG7"/>
     <mergeCell ref="CH7:CI7"/>
-    <mergeCell ref="CS5:CU5"/>
-    <mergeCell ref="BL7:BM7"/>
-    <mergeCell ref="BN7:BO7"/>
-    <mergeCell ref="BP7:BQ7"/>
-    <mergeCell ref="BR7:BS7"/>
-    <mergeCell ref="CL7:CM7"/>
-    <mergeCell ref="CN7:CO7"/>
-    <mergeCell ref="BT7:BU7"/>
-    <mergeCell ref="BV7:BW7"/>
-    <mergeCell ref="BX7:BY7"/>
-    <mergeCell ref="BZ7:CA7"/>
-    <mergeCell ref="CB7:CC7"/>
-    <mergeCell ref="CJ7:CK7"/>
-    <mergeCell ref="CD7:CE7"/>
-    <mergeCell ref="CQ6:CR8"/>
-    <mergeCell ref="CN8:CO8"/>
-    <mergeCell ref="AO6:AU6"/>
-    <mergeCell ref="AV6:BB6"/>
-    <mergeCell ref="CU6:CU9"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="BC6:BD8"/>
-    <mergeCell ref="BE6:BK6"/>
-    <mergeCell ref="BL6:CP6"/>
-    <mergeCell ref="AD7:AE7"/>
-    <mergeCell ref="AF7:AG7"/>
-    <mergeCell ref="CT6:CT9"/>
-    <mergeCell ref="BE7:BF7"/>
-    <mergeCell ref="BI7:BJ7"/>
-    <mergeCell ref="AH7:AI7"/>
-    <mergeCell ref="AJ7:AK7"/>
-    <mergeCell ref="AL7:AM7"/>
-    <mergeCell ref="AO7:AP7"/>
-    <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="AS7:AT7"/>
-    <mergeCell ref="AH8:AI8"/>
-    <mergeCell ref="BI8:BJ8"/>
-    <mergeCell ref="BL8:BM8"/>
-    <mergeCell ref="BN8:BO8"/>
-    <mergeCell ref="AL8:AM8"/>
-    <mergeCell ref="AO8:AP8"/>
-    <mergeCell ref="AQ8:AR8"/>
-    <mergeCell ref="AS8:AT8"/>
-    <mergeCell ref="BE8:BF8"/>
-    <mergeCell ref="AZ8:BA8"/>
-    <mergeCell ref="BG8:BH8"/>
-    <mergeCell ref="BZ8:CA8"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="X8:Y8"/>
-    <mergeCell ref="Z8:AA8"/>
-    <mergeCell ref="AB8:AC8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="J6:AN6"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="AF8:AG8"/>
-    <mergeCell ref="AD8:AE8"/>
-    <mergeCell ref="AJ8:AK8"/>
-    <mergeCell ref="AV8:AW8"/>
-    <mergeCell ref="AX8:AY8"/>
-    <mergeCell ref="A2:CU3"/>
-    <mergeCell ref="CB8:CC8"/>
-    <mergeCell ref="CD8:CE8"/>
-    <mergeCell ref="CF8:CG8"/>
-    <mergeCell ref="CH8:CI8"/>
-    <mergeCell ref="CJ8:CK8"/>
-    <mergeCell ref="CL8:CM8"/>
-    <mergeCell ref="BP8:BQ8"/>
-    <mergeCell ref="BR8:BS8"/>
-    <mergeCell ref="BT8:BU8"/>
-    <mergeCell ref="BV8:BW8"/>
-    <mergeCell ref="BX8:BY8"/>
   </mergeCells>
   <conditionalFormatting sqref="CU10:CU70">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
@@ -29706,106 +29706,106 @@
       <c r="F2" s="59"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="258"/>
-      <c r="B3" s="258"/>
-      <c r="C3" s="258"/>
-      <c r="D3" s="258"/>
-      <c r="E3" s="258"/>
-      <c r="F3" s="258"/>
+      <c r="A3" s="227"/>
+      <c r="B3" s="227"/>
+      <c r="C3" s="227"/>
+      <c r="D3" s="227"/>
+      <c r="E3" s="227"/>
+      <c r="F3" s="227"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="261" t="s">
+      <c r="A4" s="228" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="261"/>
-      <c r="C4" s="261"/>
-      <c r="D4" s="261"/>
-      <c r="E4" s="261"/>
-      <c r="F4" s="261"/>
+      <c r="B4" s="228"/>
+      <c r="C4" s="228"/>
+      <c r="D4" s="228"/>
+      <c r="E4" s="228"/>
+      <c r="F4" s="228"/>
     </row>
     <row r="5" spans="1:6" ht="18">
-      <c r="A5" s="262" t="s">
+      <c r="A5" s="229" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="262"/>
-      <c r="C5" s="262"/>
-      <c r="D5" s="262"/>
-      <c r="E5" s="262"/>
-      <c r="F5" s="262"/>
+      <c r="B5" s="229"/>
+      <c r="C5" s="229"/>
+      <c r="D5" s="229"/>
+      <c r="E5" s="229"/>
+      <c r="F5" s="229"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="261" t="s">
+      <c r="A6" s="228" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="261"/>
-      <c r="C6" s="261"/>
-      <c r="D6" s="261"/>
-      <c r="E6" s="261"/>
-      <c r="F6" s="261"/>
+      <c r="B6" s="228"/>
+      <c r="C6" s="228"/>
+      <c r="D6" s="228"/>
+      <c r="E6" s="228"/>
+      <c r="F6" s="228"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="263" t="s">
+      <c r="A7" s="230" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="263"/>
-      <c r="C7" s="263"/>
-      <c r="D7" s="263"/>
-      <c r="E7" s="263"/>
-      <c r="F7" s="263"/>
+      <c r="B7" s="230"/>
+      <c r="C7" s="230"/>
+      <c r="D7" s="230"/>
+      <c r="E7" s="230"/>
+      <c r="F7" s="230"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="264"/>
-      <c r="B8" s="264"/>
-      <c r="C8" s="264"/>
-      <c r="D8" s="264"/>
-      <c r="E8" s="264"/>
-      <c r="F8" s="264"/>
+      <c r="A8" s="231"/>
+      <c r="B8" s="231"/>
+      <c r="C8" s="231"/>
+      <c r="D8" s="231"/>
+      <c r="E8" s="231"/>
+      <c r="F8" s="231"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="258"/>
-      <c r="B9" s="258"/>
-      <c r="C9" s="258"/>
-      <c r="D9" s="258"/>
-      <c r="E9" s="258"/>
-      <c r="F9" s="258"/>
+      <c r="A9" s="227"/>
+      <c r="B9" s="227"/>
+      <c r="C9" s="227"/>
+      <c r="D9" s="227"/>
+      <c r="E9" s="227"/>
+      <c r="F9" s="227"/>
     </row>
     <row r="10" spans="1:6" ht="18">
-      <c r="A10" s="265"/>
-      <c r="B10" s="265"/>
-      <c r="C10" s="265"/>
-      <c r="D10" s="265"/>
-      <c r="E10" s="265"/>
-      <c r="F10" s="265"/>
+      <c r="A10" s="232"/>
+      <c r="B10" s="232"/>
+      <c r="C10" s="232"/>
+      <c r="D10" s="232"/>
+      <c r="E10" s="232"/>
+      <c r="F10" s="232"/>
     </row>
     <row r="11" spans="1:6" ht="22.5">
-      <c r="A11" s="266" t="s">
+      <c r="A11" s="233" t="s">
         <v>110</v>
       </c>
-      <c r="B11" s="266"/>
-      <c r="C11" s="266"/>
-      <c r="D11" s="266"/>
-      <c r="E11" s="266"/>
-      <c r="F11" s="266"/>
+      <c r="B11" s="233"/>
+      <c r="C11" s="233"/>
+      <c r="D11" s="233"/>
+      <c r="E11" s="233"/>
+      <c r="F11" s="233"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="264"/>
-      <c r="B12" s="264"/>
-      <c r="C12" s="264"/>
-      <c r="D12" s="264"/>
-      <c r="E12" s="264"/>
-      <c r="F12" s="264"/>
+      <c r="A12" s="231"/>
+      <c r="B12" s="231"/>
+      <c r="C12" s="231"/>
+      <c r="D12" s="231"/>
+      <c r="E12" s="231"/>
+      <c r="F12" s="231"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="59"/>
       <c r="B13" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="267" t="str">
+      <c r="C13" s="234" t="str">
         <f>REGISTRATION!C7</f>
         <v>DCIT 21</v>
       </c>
-      <c r="D13" s="267"/>
-      <c r="E13" s="267"/>
+      <c r="D13" s="234"/>
+      <c r="E13" s="234"/>
       <c r="F13" s="61"/>
     </row>
     <row r="14" spans="1:6">
@@ -29813,12 +29813,12 @@
       <c r="B14" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="260" t="str">
+      <c r="C14" s="226" t="str">
         <f>REGISTRATION!C6</f>
         <v>Programming I</v>
       </c>
-      <c r="D14" s="260"/>
-      <c r="E14" s="260"/>
+      <c r="D14" s="226"/>
+      <c r="E14" s="226"/>
       <c r="F14" s="61"/>
     </row>
     <row r="15" spans="1:6">
@@ -29826,12 +29826,12 @@
       <c r="B15" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="246" t="str">
+      <c r="C15" s="237" t="str">
         <f>REGISTRATION!A4</f>
         <v>FIRST YEAR</v>
       </c>
-      <c r="D15" s="246"/>
-      <c r="E15" s="246"/>
+      <c r="D15" s="237"/>
+      <c r="E15" s="237"/>
       <c r="F15" s="62"/>
     </row>
     <row r="16" spans="1:6">
@@ -29839,12 +29839,12 @@
       <c r="B16" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="246" t="str">
+      <c r="C16" s="237" t="str">
         <f>UPPER(CONCATENATE(REGISTRATION!C8," ",REGISTRATION!D8))</f>
         <v>IT  1A</v>
       </c>
-      <c r="D16" s="246"/>
-      <c r="E16" s="246"/>
+      <c r="D16" s="237"/>
+      <c r="E16" s="237"/>
       <c r="F16" s="62"/>
     </row>
     <row r="17" spans="1:6">
@@ -29852,12 +29852,12 @@
       <c r="B17" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="246" t="str">
+      <c r="C17" s="237" t="str">
         <f>UPPER(CONCATENATE(REGISTRATION!P13," ","SEMESTER"," ","A.Y."," ",REGISTRATION!P12))</f>
         <v>FIRST SEMESTER A.Y. 2017-2018</v>
       </c>
-      <c r="D17" s="246"/>
-      <c r="E17" s="246"/>
+      <c r="D17" s="237"/>
+      <c r="E17" s="237"/>
       <c r="F17" s="62"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1">
@@ -29869,42 +29869,42 @@
       <c r="F18" s="59"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="247" t="s">
+      <c r="A19" s="238" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="250" t="s">
+      <c r="B19" s="241" t="s">
         <v>92</v>
       </c>
-      <c r="C19" s="247" t="s">
+      <c r="C19" s="238" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="247" t="s">
+      <c r="D19" s="238" t="s">
         <v>116</v>
       </c>
-      <c r="E19" s="252" t="s">
+      <c r="E19" s="243" t="s">
         <v>117</v>
       </c>
-      <c r="F19" s="247" t="s">
+      <c r="F19" s="238" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="248"/>
-      <c r="B20" s="251"/>
-      <c r="C20" s="248"/>
-      <c r="D20" s="248"/>
-      <c r="E20" s="253"/>
-      <c r="F20" s="255"/>
+      <c r="A20" s="239"/>
+      <c r="B20" s="242"/>
+      <c r="C20" s="239"/>
+      <c r="D20" s="239"/>
+      <c r="E20" s="244"/>
+      <c r="F20" s="246"/>
     </row>
     <row r="21" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A21" s="249"/>
+      <c r="A21" s="240"/>
       <c r="B21" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="C21" s="249"/>
-      <c r="D21" s="249"/>
-      <c r="E21" s="254"/>
-      <c r="F21" s="256"/>
+      <c r="C21" s="240"/>
+      <c r="D21" s="240"/>
+      <c r="E21" s="245"/>
+      <c r="F21" s="247"/>
     </row>
     <row r="22" spans="1:6" ht="18">
       <c r="A22" s="64">
@@ -31417,14 +31417,14 @@
       <c r="F82" s="83"/>
     </row>
     <row r="83" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A83" s="230" t="s">
+      <c r="A83" s="254" t="s">
         <v>119</v>
       </c>
-      <c r="B83" s="231"/>
-      <c r="C83" s="231"/>
-      <c r="D83" s="231"/>
-      <c r="E83" s="231"/>
-      <c r="F83" s="232"/>
+      <c r="B83" s="255"/>
+      <c r="C83" s="255"/>
+      <c r="D83" s="255"/>
+      <c r="E83" s="255"/>
+      <c r="F83" s="256"/>
     </row>
     <row r="84" spans="1:6" ht="15.75">
       <c r="A84" s="61"/>
@@ -31457,11 +31457,11 @@
       </c>
       <c r="C87" s="59"/>
       <c r="D87" s="59"/>
-      <c r="E87" s="257">
+      <c r="E87" s="248">
         <f ca="1">NOW()</f>
-        <v>43022.327739930559</v>
-      </c>
-      <c r="F87" s="257"/>
+        <v>43023.817172222225</v>
+      </c>
+      <c r="F87" s="248"/>
     </row>
     <row r="88" spans="1:6" ht="15.75">
       <c r="A88" s="59"/>
@@ -31471,10 +31471,10 @@
       </c>
       <c r="C88" s="72"/>
       <c r="D88" s="72"/>
-      <c r="E88" s="258" t="s">
+      <c r="E88" s="227" t="s">
         <v>121</v>
       </c>
-      <c r="F88" s="258"/>
+      <c r="F88" s="227"/>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="59"/>
@@ -31491,8 +31491,8 @@
       <c r="B90" s="73"/>
       <c r="C90" s="73"/>
       <c r="D90" s="73"/>
-      <c r="E90" s="258"/>
-      <c r="F90" s="258"/>
+      <c r="E90" s="227"/>
+      <c r="F90" s="227"/>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="59"/>
@@ -31608,14 +31608,14 @@
       <c r="F104" s="59"/>
     </row>
     <row r="105" spans="1:7" ht="15.75">
-      <c r="A105" s="259" t="s">
+      <c r="A105" s="249" t="s">
         <v>136</v>
       </c>
-      <c r="B105" s="259"/>
-      <c r="C105" s="259"/>
-      <c r="D105" s="259"/>
-      <c r="E105" s="259"/>
-      <c r="F105" s="259"/>
+      <c r="B105" s="249"/>
+      <c r="C105" s="249"/>
+      <c r="D105" s="249"/>
+      <c r="E105" s="249"/>
+      <c r="F105" s="249"/>
     </row>
     <row r="106" spans="1:7" ht="15.75" thickBot="1">
       <c r="A106" s="59"/>
@@ -31630,124 +31630,124 @@
       <c r="B107" s="77" t="s">
         <v>137</v>
       </c>
-      <c r="C107" s="243" t="s">
+      <c r="C107" s="267" t="s">
         <v>138</v>
       </c>
-      <c r="D107" s="244"/>
-      <c r="E107" s="245" t="s">
+      <c r="D107" s="236"/>
+      <c r="E107" s="235" t="s">
         <v>139</v>
       </c>
-      <c r="F107" s="244"/>
+      <c r="F107" s="236"/>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="59"/>
       <c r="B108" s="85" t="s">
         <v>123</v>
       </c>
-      <c r="C108" s="239">
+      <c r="C108" s="263">
         <f>COUNTIF($D$22:$D$82,"=1.0")+COUNTIF($D$22:$D$82,"=1.25")+(COUNTIF($D$22:$D$82,"=1.50")+COUNTIF($D$22:$D$82,"=1.75"))</f>
         <v>0</v>
       </c>
-      <c r="D108" s="240"/>
-      <c r="E108" s="241">
+      <c r="D108" s="264"/>
+      <c r="E108" s="265">
         <f>(C108/$C$114)*100</f>
         <v>0</v>
       </c>
-      <c r="F108" s="242"/>
+      <c r="F108" s="266"/>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" s="59"/>
       <c r="B109" s="86" t="s">
         <v>124</v>
       </c>
-      <c r="C109" s="233">
+      <c r="C109" s="257">
         <f>COUNTIF($D$22:$D$82,"=2.0")+COUNTIF($D$22:$D$82,"=2.25")+(COUNTIF($D$22:$D$82,"=2.50")+COUNTIF($D$22:$D$82,"=2.75"))</f>
         <v>0</v>
       </c>
-      <c r="D109" s="234"/>
-      <c r="E109" s="235">
+      <c r="D109" s="258"/>
+      <c r="E109" s="259">
         <f>(C109/$C$114)*100</f>
         <v>0</v>
       </c>
-      <c r="F109" s="236"/>
+      <c r="F109" s="260"/>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="59"/>
       <c r="B110" s="86" t="s">
         <v>125</v>
       </c>
-      <c r="C110" s="233">
+      <c r="C110" s="257">
         <f>COUNTIF($D$22:$D$82,"=3.0")</f>
         <v>0</v>
       </c>
-      <c r="D110" s="234"/>
-      <c r="E110" s="235">
+      <c r="D110" s="258"/>
+      <c r="E110" s="259">
         <f t="shared" ref="E110:E113" si="1">(C110/$C$114)*100</f>
         <v>0</v>
       </c>
-      <c r="F110" s="236"/>
+      <c r="F110" s="260"/>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="59"/>
       <c r="B111" s="86" t="s">
         <v>126</v>
       </c>
-      <c r="C111" s="233">
+      <c r="C111" s="257">
         <f>COUNTIF($D$22:$D$82,"=5.0")</f>
         <v>60</v>
       </c>
-      <c r="D111" s="234"/>
-      <c r="E111" s="235">
+      <c r="D111" s="258"/>
+      <c r="E111" s="259">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="F111" s="236"/>
+      <c r="F111" s="260"/>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="59"/>
       <c r="B112" s="86" t="s">
         <v>127</v>
       </c>
-      <c r="C112" s="237">
-        <v>0</v>
-      </c>
-      <c r="D112" s="238"/>
-      <c r="E112" s="235">
+      <c r="C112" s="261">
+        <v>0</v>
+      </c>
+      <c r="D112" s="262"/>
+      <c r="E112" s="259">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F112" s="236"/>
+      <c r="F112" s="260"/>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" s="59"/>
       <c r="B113" s="86" t="s">
         <v>128</v>
       </c>
-      <c r="C113" s="237">
-        <v>0</v>
-      </c>
-      <c r="D113" s="238"/>
-      <c r="E113" s="235">
+      <c r="C113" s="261">
+        <v>0</v>
+      </c>
+      <c r="D113" s="262"/>
+      <c r="E113" s="259">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F113" s="236"/>
+      <c r="F113" s="260"/>
     </row>
     <row r="114" spans="1:6" ht="16.5" thickBot="1">
       <c r="A114" s="59"/>
       <c r="B114" s="87" t="s">
         <v>129</v>
       </c>
-      <c r="C114" s="226">
+      <c r="C114" s="250">
         <f>SUM(C108:D113)</f>
         <v>60</v>
       </c>
-      <c r="D114" s="227"/>
-      <c r="E114" s="228">
+      <c r="D114" s="251"/>
+      <c r="E114" s="252">
         <f>SUM(E108:F113)</f>
         <v>100</v>
       </c>
-      <c r="F114" s="229"/>
+      <c r="F114" s="253"/>
     </row>
     <row r="115" spans="1:6">
       <c r="A115" s="59"/>
@@ -31915,32 +31915,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="42">
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="E107:F107"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="E87:F87"/>
-    <mergeCell ref="E88:F88"/>
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="A105:F105"/>
     <mergeCell ref="C114:D114"/>
     <mergeCell ref="E114:F114"/>
     <mergeCell ref="A83:F83"/>
@@ -31957,6 +31931,32 @@
     <mergeCell ref="C110:D110"/>
     <mergeCell ref="E110:F110"/>
     <mergeCell ref="C107:D107"/>
+    <mergeCell ref="E107:F107"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="E87:F87"/>
+    <mergeCell ref="E88:F88"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="A105:F105"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="C13:E13"/>
   </mergeCells>
   <conditionalFormatting sqref="F22:F81">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>

<commit_message>
Quiz 3 and 4 DCIT 21 Updates
</commit_message>
<xml_diff>
--- a/DCIT 21 - IT 1A/LEC AND LAB - IT 1A.xlsx
+++ b/DCIT 21 - IT 1A/LEC AND LAB - IT 1A.xlsx
@@ -8731,9 +8731,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:CU70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O40" sqref="O40"/>
+      <selection pane="topRight" activeCell="J7" sqref="J7:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9213,7 +9213,9 @@
         <v>43046</v>
       </c>
       <c r="O7" s="185"/>
-      <c r="P7" s="185"/>
+      <c r="P7" s="185">
+        <v>43063</v>
+      </c>
       <c r="Q7" s="185"/>
       <c r="R7" s="185"/>
       <c r="S7" s="185"/>
@@ -15305,16 +15307,18 @@
         <v>45.714285714285715</v>
       </c>
       <c r="N30" s="101">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="O30" s="85">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P30" s="101"/>
+        <v>100</v>
+      </c>
+      <c r="P30" s="101">
+        <v>2</v>
+      </c>
       <c r="Q30" s="85">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>13.333333333333334</v>
       </c>
       <c r="R30" s="101"/>
       <c r="S30" s="85" t="str">
@@ -15346,7 +15350,7 @@
       <c r="AM30" s="87"/>
       <c r="AN30" s="88">
         <f t="shared" si="9"/>
-        <v>6.7857142857142865</v>
+        <v>12.452380952380954</v>
       </c>
       <c r="AO30" s="101">
         <v>70</v>
@@ -15392,11 +15396,11 @@
       </c>
       <c r="BC30" s="91">
         <f t="shared" si="18"/>
-        <v>43.928571428571431</v>
+        <v>49.595238095238102</v>
       </c>
       <c r="BD30" s="91">
         <f t="shared" si="19"/>
-        <v>43.93</v>
+        <v>49.6</v>
       </c>
       <c r="BE30" s="101"/>
       <c r="BF30" s="85">
@@ -15520,7 +15524,7 @@
       </c>
       <c r="CS30" s="97">
         <f t="shared" si="45"/>
-        <v>35.271999999999998</v>
+        <v>37.540000000000006</v>
       </c>
       <c r="CT30" s="97">
         <f>IFERROR(VLOOKUP(CS30,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -17771,13 +17775,15 @@
         <v>45.714285714285715</v>
       </c>
       <c r="N39" s="101">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O39" s="85">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P39" s="101"/>
+        <v>22.857142857142858</v>
+      </c>
+      <c r="P39" s="101">
+        <v>0</v>
+      </c>
       <c r="Q39" s="85">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -17812,7 +17818,7 @@
       <c r="AM39" s="87"/>
       <c r="AN39" s="88">
         <f t="shared" si="9"/>
-        <v>7.0357142857142865</v>
+        <v>8.1785714285714288</v>
       </c>
       <c r="AO39" s="101">
         <v>70</v>
@@ -17858,11 +17864,11 @@
       </c>
       <c r="BC39" s="91">
         <f t="shared" si="18"/>
-        <v>44.607142857142854</v>
+        <v>45.75</v>
       </c>
       <c r="BD39" s="91">
         <f t="shared" si="19"/>
-        <v>44.61</v>
+        <v>45.75</v>
       </c>
       <c r="BE39" s="101"/>
       <c r="BF39" s="85">
@@ -17988,7 +17994,7 @@
       </c>
       <c r="CS39" s="97">
         <f t="shared" si="45"/>
-        <v>38.094000000000001</v>
+        <v>38.549999999999997</v>
       </c>
       <c r="CT39" s="97">
         <f>IFERROR(VLOOKUP(CS39,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -19705,11 +19711,11 @@
         <v>42.857142857142854</v>
       </c>
       <c r="N46" s="101">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O46" s="85">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>17.142857142857142</v>
       </c>
       <c r="P46" s="101"/>
       <c r="Q46" s="85">
@@ -19746,7 +19752,7 @@
       <c r="AM46" s="87"/>
       <c r="AN46" s="88">
         <f t="shared" si="9"/>
-        <v>6.6428571428571432</v>
+        <v>7.5</v>
       </c>
       <c r="AO46" s="101">
         <v>70</v>
@@ -19792,11 +19798,11 @@
       </c>
       <c r="BC46" s="91">
         <f t="shared" si="18"/>
-        <v>43.785714285714285</v>
+        <v>44.642857142857139</v>
       </c>
       <c r="BD46" s="91">
         <f t="shared" si="19"/>
-        <v>43.79</v>
+        <v>44.64</v>
       </c>
       <c r="BE46" s="101"/>
       <c r="BF46" s="85">
@@ -19920,7 +19926,7 @@
       </c>
       <c r="CS46" s="97">
         <f t="shared" si="45"/>
-        <v>35.216000000000001</v>
+        <v>35.555999999999997</v>
       </c>
       <c r="CT46" s="97">
         <f>IFERROR(VLOOKUP(CS46,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -23589,10 +23595,12 @@
         <f t="shared" si="5"/>
         <v>22.857142857142858</v>
       </c>
-      <c r="P60" s="101"/>
+      <c r="P60" s="101">
+        <v>11</v>
+      </c>
       <c r="Q60" s="85">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>73.333333333333329</v>
       </c>
       <c r="R60" s="101"/>
       <c r="S60" s="85" t="str">
@@ -23624,7 +23632,7 @@
       <c r="AM60" s="87"/>
       <c r="AN60" s="88">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>11.666666666666666</v>
       </c>
       <c r="AO60" s="101">
         <v>50</v>
@@ -23670,11 +23678,11 @@
       </c>
       <c r="BC60" s="91">
         <f t="shared" si="18"/>
-        <v>47</v>
+        <v>50.666666666666664</v>
       </c>
       <c r="BD60" s="91">
         <f t="shared" si="19"/>
-        <v>47</v>
+        <v>50.67</v>
       </c>
       <c r="BE60" s="101"/>
       <c r="BF60" s="85">
@@ -23784,7 +23792,7 @@
       </c>
       <c r="CS60" s="97">
         <f t="shared" si="45"/>
-        <v>18.8</v>
+        <v>20.268000000000001</v>
       </c>
       <c r="CT60" s="97">
         <f>IFERROR(VLOOKUP(CS60,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -27885,7 +27893,7 @@
       </c>
       <c r="E28" s="51">
         <f>'RAW GRADES'!AN30</f>
-        <v>6.7857142857142865</v>
+        <v>12.452380952380954</v>
       </c>
       <c r="F28" s="51">
         <f>'RAW GRADES'!AU30</f>
@@ -27897,11 +27905,11 @@
       </c>
       <c r="H28" s="52">
         <f>'RAW GRADES'!BC30</f>
-        <v>43.928571428571431</v>
+        <v>49.595238095238102</v>
       </c>
       <c r="I28" s="52">
         <f>'RAW GRADES'!BD30</f>
-        <v>43.93</v>
+        <v>49.6</v>
       </c>
       <c r="J28" s="51">
         <f>'RAW GRADES'!BK30</f>
@@ -27921,7 +27929,7 @@
       </c>
       <c r="N28" s="57">
         <f>'RAW GRADES'!CS30</f>
-        <v>35.271999999999998</v>
+        <v>37.540000000000006</v>
       </c>
       <c r="O28" s="55">
         <f>'RAW GRADES'!CT30</f>
@@ -28468,7 +28476,7 @@
       </c>
       <c r="E37" s="51">
         <f>'RAW GRADES'!AN39</f>
-        <v>7.0357142857142865</v>
+        <v>8.1785714285714288</v>
       </c>
       <c r="F37" s="51">
         <f>'RAW GRADES'!AU39</f>
@@ -28480,11 +28488,11 @@
       </c>
       <c r="H37" s="52">
         <f>'RAW GRADES'!BC39</f>
-        <v>44.607142857142854</v>
+        <v>45.75</v>
       </c>
       <c r="I37" s="52">
         <f>'RAW GRADES'!BD39</f>
-        <v>44.61</v>
+        <v>45.75</v>
       </c>
       <c r="J37" s="51">
         <f>'RAW GRADES'!BK39</f>
@@ -28504,7 +28512,7 @@
       </c>
       <c r="N37" s="57">
         <f>'RAW GRADES'!CS39</f>
-        <v>38.094000000000001</v>
+        <v>38.549999999999997</v>
       </c>
       <c r="O37" s="55">
         <f>'RAW GRADES'!CT39</f>
@@ -28923,7 +28931,7 @@
       </c>
       <c r="E44" s="51">
         <f>'RAW GRADES'!AN46</f>
-        <v>6.6428571428571432</v>
+        <v>7.5</v>
       </c>
       <c r="F44" s="51">
         <f>'RAW GRADES'!AU46</f>
@@ -28935,11 +28943,11 @@
       </c>
       <c r="H44" s="52">
         <f>'RAW GRADES'!BC46</f>
-        <v>43.785714285714285</v>
+        <v>44.642857142857139</v>
       </c>
       <c r="I44" s="52">
         <f>'RAW GRADES'!BD46</f>
-        <v>43.79</v>
+        <v>44.64</v>
       </c>
       <c r="J44" s="51">
         <f>'RAW GRADES'!BK46</f>
@@ -28959,7 +28967,7 @@
       </c>
       <c r="N44" s="57">
         <f>'RAW GRADES'!CS46</f>
-        <v>35.216000000000001</v>
+        <v>35.555999999999997</v>
       </c>
       <c r="O44" s="55">
         <f>'RAW GRADES'!CT46</f>
@@ -29833,7 +29841,7 @@
       </c>
       <c r="E58" s="51">
         <f>'RAW GRADES'!AN60</f>
-        <v>8</v>
+        <v>11.666666666666666</v>
       </c>
       <c r="F58" s="51">
         <f>'RAW GRADES'!AU60</f>
@@ -29845,11 +29853,11 @@
       </c>
       <c r="H58" s="52">
         <f>'RAW GRADES'!BC60</f>
-        <v>47</v>
+        <v>50.666666666666664</v>
       </c>
       <c r="I58" s="52">
         <f>'RAW GRADES'!BD60</f>
-        <v>47</v>
+        <v>50.67</v>
       </c>
       <c r="J58" s="51">
         <f>'RAW GRADES'!BK60</f>
@@ -29869,7 +29877,7 @@
       </c>
       <c r="N58" s="57">
         <f>'RAW GRADES'!CS60</f>
-        <v>18.8</v>
+        <v>20.268000000000001</v>
       </c>
       <c r="O58" s="55">
         <f>'RAW GRADES'!CT60</f>
@@ -32105,7 +32113,7 @@
       <c r="D77" s="59"/>
       <c r="E77" s="251">
         <f ca="1">NOW()</f>
-        <v>43067.733531365739</v>
+        <v>43070.580560069444</v>
       </c>
       <c r="F77" s="251"/>
       <c r="G77" s="123"/>

</xml_diff>